<commit_message>
added all new test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/Test_Data_Sheet.xlsx
+++ b/src/test/resources/testdata/Test_Data_Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sunil\eclipse-workspace\Regression_Pos_project\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7AA98DD-1D47-4509-8ADC-D5F99F306E76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{009BA1F3-C5C8-4694-ADDB-269286632F7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{52826312-55BE-45F7-9B29-2F6A9A52A5DF}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="100">
   <si>
     <t>admin</t>
   </si>
@@ -169,9 +169,6 @@
     <t>ajith.h@proenx.com</t>
   </si>
   <si>
-    <t>TestPractice4</t>
-  </si>
-  <si>
     <t>Rdep Meta Limited Pune - 1765</t>
   </si>
   <si>
@@ -185,13 +182,169 @@
   </si>
   <si>
     <t>2024-05-10 04:51 pm</t>
+  </si>
+  <si>
+    <t>Master Promotion End Date Format</t>
+  </si>
+  <si>
+    <t>Master Promotion Start Date Format</t>
+  </si>
+  <si>
+    <t>Active Status1</t>
+  </si>
+  <si>
+    <t>Active Status2</t>
+  </si>
+  <si>
+    <t>just check</t>
+  </si>
+  <si>
+    <t>sunil</t>
+  </si>
+  <si>
+    <t>trail</t>
+  </si>
+  <si>
+    <t>sunil2</t>
+  </si>
+  <si>
+    <t>2024-10-03 04:51 pm</t>
+  </si>
+  <si>
+    <t>2024-02-10 04:51 pm</t>
+  </si>
+  <si>
+    <t>PromotionTestCase1</t>
+  </si>
+  <si>
+    <t>Sr. No</t>
+  </si>
+  <si>
+    <t>Run Mode</t>
+  </si>
+  <si>
+    <t>Testing _Type</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Regression</t>
+  </si>
+  <si>
+    <t>Smoke</t>
+  </si>
+  <si>
+    <t>Sanity</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>Inprogress</t>
+  </si>
+  <si>
+    <t>Non-Started</t>
+  </si>
+  <si>
+    <t>TestPractice3</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Test_Case_Name</t>
+  </si>
+  <si>
+    <t>Create_SimpleLine_Promo_System</t>
+  </si>
+  <si>
+    <t>2024-10-05 04:51 pm</t>
+  </si>
+  <si>
+    <t>2024-10-07 04:51 pm</t>
+  </si>
+  <si>
+    <t>Promotion Type1</t>
+  </si>
+  <si>
+    <t>Simple Line</t>
+  </si>
+  <si>
+    <t>Flat 10% OFF</t>
+  </si>
+  <si>
+    <t>Promotion Type2</t>
+  </si>
+  <si>
+    <t>Promotion Type3</t>
+  </si>
+  <si>
+    <t>Promotion Type4</t>
+  </si>
+  <si>
+    <t>Promotion Type5</t>
+  </si>
+  <si>
+    <t>Promotion Type6</t>
+  </si>
+  <si>
+    <t>Promotion Type7</t>
+  </si>
+  <si>
+    <t>Promotion Sub type1</t>
+  </si>
+  <si>
+    <t>Percentage</t>
+  </si>
+  <si>
+    <t>Promotion Code</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Discount Value</t>
+  </si>
+  <si>
+    <t>F10%</t>
+  </si>
+  <si>
+    <t>Simple Line Promotion</t>
+  </si>
+  <si>
+    <t>Promotion Name</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Promotion successful Message</t>
+  </si>
+  <si>
+    <t>Promotion configured successfully</t>
+  </si>
+  <si>
+    <t>Promotion Details Error PopUp</t>
+  </si>
+  <si>
+    <t>Please Select Promotion Type</t>
+  </si>
+  <si>
+    <t>Coupon Field</t>
+  </si>
+  <si>
+    <t>T20WC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,8 +366,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -229,12 +388,42 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor theme="3" tint="0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -242,20 +431,59 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="22" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="22" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -591,46 +819,131 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.7265625" style="11"/>
+    <col min="2" max="2" width="29.26953125" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7265625" style="13"/>
+    <col min="4" max="4" width="11.54296875" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6328125" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.7265625" style="16"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="11">
+        <v>1</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="11">
+        <v>2</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="11">
+        <v>3</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="11">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
+      <c r="B5" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{0B33546C-2E36-4AF5-B702-4D0334972A35}">
+      <formula1>"Y,N"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576" xr:uid="{AEBF9179-D691-4AFE-9C0F-7B9ECE5923E0}">
+      <formula1>"Complete,Inprogress,Non-Started"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Y7"/>
+  <dimension ref="A1:Y15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.453125" customWidth="1"/>
     <col min="4" max="4" width="11.81640625" customWidth="1"/>
@@ -644,8 +957,8 @@
     <col min="14" max="14" width="26" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="25" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.81640625" customWidth="1"/>
-    <col min="18" max="18" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="28.81640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="25.6328125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="13" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="20.7265625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="31.81640625" bestFit="1" customWidth="1"/>
@@ -656,7 +969,7 @@
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="7"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -705,10 +1018,10 @@
         <v>24</v>
       </c>
       <c r="P2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q2" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="R2" s="2" t="s">
         <v>26</v>
@@ -772,20 +1085,20 @@
       <c r="L3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="M3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="N3" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="O3" s="4" t="s">
+      <c r="N3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="O3" s="3" t="s">
         <v>31</v>
       </c>
       <c r="P3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q3" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="R3" s="2" t="s">
         <v>27</v>
@@ -796,88 +1109,392 @@
       <c r="T3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="U3" s="5" t="s">
+      <c r="U3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="V3" s="5" t="s">
+      <c r="V3" s="4" t="s">
         <v>32</v>
       </c>
       <c r="W3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="X3" s="5" t="s">
+      <c r="X3" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="Y3" s="6" t="s">
+      <c r="Y3" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:25" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="N6" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="O6" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="L7" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="M7" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="N7" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="O7" s="8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="U10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="V10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="W10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="X10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y10" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="P11" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+      <c r="Q11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="U11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="V11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="W11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="X11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y11" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A13" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B14" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+      <c r="C14" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="L14" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="M14" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="N14" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="O14" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="P14" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q14" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="R14" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="S14" s="8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B15" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>14</v>
+      <c r="C15" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="J15" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="K15" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="L15" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="M15" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="N15" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="O15" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="P15" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q15" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="R15" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="S15" s="8" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="Y3" r:id="rId1" xr:uid="{2F8DBC2D-3C9E-4C2E-89A8-68E0ACD71B93}"/>
+    <hyperlink ref="Y11" r:id="rId2" xr:uid="{3EE8ECB8-9837-4CC6-9076-C1C8D65F5572}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
test case update for jenkins
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/Test_Data_Sheet.xlsx
+++ b/src/test/resources/testdata/Test_Data_Sheet.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sunil\eclipse-workspace\Regression_Pos_project\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3F37D09-2424-47CF-96A8-E2A426845BF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB7A85F-CFEB-495B-AB72-3A07E5A00E65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{52826312-55BE-45F7-9B29-2F6A9A52A5DF}"/>
+    <workbookView xWindow="3590" yWindow="0" windowWidth="15610" windowHeight="10080" xr2:uid="{52826312-55BE-45F7-9B29-2F6A9A52A5DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="2" r:id="rId1"/>
-    <sheet name="Test Sunil" sheetId="3" r:id="rId2"/>
-    <sheet name="PROENX" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId2"/>
+    <sheet name="Test Sunil" sheetId="3" r:id="rId3"/>
+    <sheet name="PROENX" sheetId="4" r:id="rId4"/>
+    <sheet name="QA Set" sheetId="5" r:id="rId5"/>
+    <sheet name="UAT Set" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1248" uniqueCount="257">
   <si>
     <t>admin</t>
   </si>
@@ -203,12 +205,6 @@
     <t>sunil</t>
   </si>
   <si>
-    <t>trail</t>
-  </si>
-  <si>
-    <t>sunil2</t>
-  </si>
-  <si>
     <t>2024-10-03 04:51 pm</t>
   </si>
   <si>
@@ -501,6 +497,321 @@
   </si>
   <si>
     <t>Select All</t>
+  </si>
+  <si>
+    <t>Inventory List Store Name1</t>
+  </si>
+  <si>
+    <t>Inventory List Store Name2</t>
+  </si>
+  <si>
+    <t>Inventory List Store Name3</t>
+  </si>
+  <si>
+    <t>Inventory_TestCases</t>
+  </si>
+  <si>
+    <t>sky</t>
+  </si>
+  <si>
+    <t>wwe</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>Inventory Adjustment Successful Message</t>
+  </si>
+  <si>
+    <t>Inventory Adjustment Unsuccessful Message</t>
+  </si>
+  <si>
+    <t>Error updating inventory.</t>
+  </si>
+  <si>
+    <t>Inventory adjusted successfully.</t>
+  </si>
+  <si>
+    <t>Inventory Adjustment Error Message for not selecting Store</t>
+  </si>
+  <si>
+    <t>Inventory Adjustment Error Message for not selecting file</t>
+  </si>
+  <si>
+    <t>Please Select Store</t>
+  </si>
+  <si>
+    <t>Please Select File</t>
+  </si>
+  <si>
+    <t>Inventory Import Store</t>
+  </si>
+  <si>
+    <t>Inventory Import Successful Message</t>
+  </si>
+  <si>
+    <t>Inventory Import Unsuccessful Message</t>
+  </si>
+  <si>
+    <t>Inventory imported successfully.</t>
+  </si>
+  <si>
+    <t>Inventory Import Error Message for not selecting Store</t>
+  </si>
+  <si>
+    <t>Inventory Import Error Message for not selecting file</t>
+  </si>
+  <si>
+    <t>Required data not found. Please upload the correct file.</t>
+  </si>
+  <si>
+    <t>Inventory List Filter Select Store1</t>
+  </si>
+  <si>
+    <t>Inventory List Search Data for Update1</t>
+  </si>
+  <si>
+    <t>Inventory List Search Data for File Reset1</t>
+  </si>
+  <si>
+    <t>Inventory List Search Data for File Reset2</t>
+  </si>
+  <si>
+    <t>Inventory List Search Data for File Reset3</t>
+  </si>
+  <si>
+    <t>50002201</t>
+  </si>
+  <si>
+    <t>50002202</t>
+  </si>
+  <si>
+    <t>Inventory List Search Data for Update2</t>
+  </si>
+  <si>
+    <t>Inventory List Search Data for Update3</t>
+  </si>
+  <si>
+    <t>8904389909669</t>
+  </si>
+  <si>
+    <t>Edit Inventory Reorder Threshold Value</t>
+  </si>
+  <si>
+    <t>Edit Inventory Inventory Update Reason</t>
+  </si>
+  <si>
+    <t>Testing Purpose</t>
+  </si>
+  <si>
+    <t>Inventory updated.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edit Inventory Successful Message </t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Inventory List Search SKU for Edit Inventory</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Table data Verification</t>
+  </si>
+  <si>
+    <t>1234RDEP</t>
+  </si>
+  <si>
+    <t>Product Sku</t>
+  </si>
+  <si>
+    <t>Product Name</t>
+  </si>
+  <si>
+    <t>Cotton Jeans 6 Packet</t>
+  </si>
+  <si>
+    <t>Product Description</t>
+  </si>
+  <si>
+    <t>Pure cotton with Sky Blue Color</t>
+  </si>
+  <si>
+    <t>Select Store for adding new Product</t>
+  </si>
+  <si>
+    <t>Single_Product_TestCases</t>
+  </si>
+  <si>
+    <t>Blissclub HSR - 0265</t>
+  </si>
+  <si>
+    <t>Select Category for adding new Product</t>
+  </si>
+  <si>
+    <t>Mens</t>
+  </si>
+  <si>
+    <t>Attribute Type1</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>Attribute Value1</t>
+  </si>
+  <si>
+    <t>Bella Blue</t>
+  </si>
+  <si>
+    <t>399</t>
+  </si>
+  <si>
+    <t>Unit Price for adding new Product</t>
+  </si>
+  <si>
+    <t>Least Price for adding new Product</t>
+  </si>
+  <si>
+    <t>Stock for adding new Product</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Catagory Name inside Add Catagory Screen</t>
+  </si>
+  <si>
+    <t>Catagory Description inside Add Catagory Screen</t>
+  </si>
+  <si>
+    <t>Pure Cotton with HandMade Craft</t>
+  </si>
+  <si>
+    <t>Select Store for adding new Catagory</t>
+  </si>
+  <si>
+    <t>Please Enter Product SKU.</t>
+  </si>
+  <si>
+    <t>Error Message for  Product SKU Mandatory Field</t>
+  </si>
+  <si>
+    <t>Please Enter Product Name</t>
+  </si>
+  <si>
+    <t>Error Message for  Product Name Mandatory Field</t>
+  </si>
+  <si>
+    <t>Please Select Store.</t>
+  </si>
+  <si>
+    <t>Error Message for  Select Store Mandatory Field</t>
+  </si>
+  <si>
+    <t>Please Enter Category Name</t>
+  </si>
+  <si>
+    <t>Error Message for   Entering Category Name  Mandatory Field</t>
+  </si>
+  <si>
+    <t>Error Message for   Entering Description  Mandatory Field</t>
+  </si>
+  <si>
+    <t>Please Enter Category Description</t>
+  </si>
+  <si>
+    <t>Cotton Section1</t>
+  </si>
+  <si>
+    <t>BlissClub Store Demo HSR - 0269</t>
+  </si>
+  <si>
+    <t>3456RDEP</t>
+  </si>
+  <si>
+    <t>Cotton Jeans Denim Packet</t>
+  </si>
+  <si>
+    <t>599</t>
+  </si>
+  <si>
+    <t>Cotton Section2</t>
+  </si>
+  <si>
+    <t>Please Select Category.</t>
+  </si>
+  <si>
+    <t>Error Message for  Product Catagory  Mandatory Field</t>
+  </si>
+  <si>
+    <t>1616204001002</t>
+  </si>
+  <si>
+    <t>Inventory List Search Data for Update for three sku1</t>
+  </si>
+  <si>
+    <t>Inventory List Search Data for Update for three sku2</t>
+  </si>
+  <si>
+    <t>Inventory List Search Data for Update for three sku3</t>
+  </si>
+  <si>
+    <t>50002200</t>
+  </si>
+  <si>
+    <t>80002500</t>
+  </si>
+  <si>
+    <t>60002300</t>
+  </si>
+  <si>
+    <t>Inventory List Search Data for File Reset with Single SKU file</t>
+  </si>
+  <si>
+    <t>Inventory List Search Data forUpdate with Single SKU file</t>
+  </si>
+  <si>
+    <t>Inventory List Search Data for File Reset for three sku1</t>
+  </si>
+  <si>
+    <t>Inventory List Search Data for File Reset for three sku2</t>
+  </si>
+  <si>
+    <t>Inventory List Search Data for File Reset for three sku3</t>
+  </si>
+  <si>
+    <t>8904389900567</t>
+  </si>
+  <si>
+    <t>8904389900550</t>
+  </si>
+  <si>
+    <t>70002400</t>
+  </si>
+  <si>
+    <t>40002100</t>
+  </si>
+  <si>
+    <t>202325_Glass_Bottle</t>
+  </si>
+  <si>
+    <t>202325</t>
+  </si>
+  <si>
+    <t>Pure Crystal Glass Boltle withEnv Friendlt Material</t>
+  </si>
+  <si>
+    <t>Accessories</t>
+  </si>
+  <si>
+    <t>C:\\Users\\sunil\\Test File Format\\screenshot.png</t>
+  </si>
+  <si>
+    <t>path of file</t>
   </si>
 </sst>
 </file>
@@ -536,7 +847,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -591,6 +902,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -620,7 +937,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -661,6 +978,11 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="22" fontId="0" fillId="9" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -996,10 +1318,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1014,19 +1336,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="C1" s="13" t="s">
+      <c r="E1" s="15" t="s">
         <v>60</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -1034,16 +1356,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>69</v>
+        <v>191</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -1054,13 +1376,13 @@
         <v>3</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>69</v>
+        <v>191</v>
       </c>
       <c r="D3" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="15" t="s">
         <v>64</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -1068,16 +1390,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>69</v>
+        <v>191</v>
       </c>
       <c r="D4" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="15" t="s">
         <v>65</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -1085,16 +1407,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>69</v>
+        <v>191</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -1102,16 +1424,50 @@
         <v>5</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>69</v>
+        <v>191</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E6" s="15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="11">
+        <v>6</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="11">
+        <v>7</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="C8" s="13" t="s">
         <v>67</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1128,11 +1484,1501 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F95DBB38-CB29-429B-8643-7E9E0FC99A14}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="11">
+        <v>7</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="11">
+        <v>1</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="11">
+        <v>2</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="11">
+        <v>3</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="11">
+        <v>4</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="11">
+        <v>5</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E6" xr:uid="{CA7B4B4D-3034-4F4A-8B87-FCCD8D28759A}">
+      <formula1>"Complete,Inprogress,Non-Started"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C6" xr:uid="{CD124A89-850C-47D5-9AAD-BFA94E434699}">
+      <formula1>"Y,N"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AR23"/>
+  <dimension ref="A1:AR31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="33.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="22.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="48.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="46.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.90625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="44.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="42.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="45.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="34.08984375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="32" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="41.36328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="40.54296875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="30.26953125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="28.81640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="25.90625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="29.81640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="31.81640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="32.36328125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="26.08984375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="27" max="31" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="30.36328125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="29.453125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="28.81640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="25.6328125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="25.90625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="11.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="6"/>
+    </row>
+    <row r="2" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="V3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="X3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y3" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="N6" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="O6" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="P6" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q6" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="R6" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="S6" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="T6" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="U6" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="V6" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="W6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="X6" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="L7" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="N7" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="O7" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="P7" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q7" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="R7" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="S7" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="T7" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="U7" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="V7" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="W7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="X7" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="U10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="V10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="W10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="X10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y10" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="U11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="V11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="W11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="X11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y11" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A13" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="L14" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="M14" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="N14" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="O14" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="P14" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q14" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="R14" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="S14" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="T14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="U14" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="K15" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="L15" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="M15" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="N15" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="O15" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="P15" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q15" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="R15" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="S15" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="T15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="U15" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:44" s="19" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="18" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:44" s="19" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="G18" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="H18" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="I18" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="J18" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="K18" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="L18" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="M18" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="N18" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="O18" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="P18" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q18" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="R18" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="S18" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="T18" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="U18" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="V18" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="W18" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="X18" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y18" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z18" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA18" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB18" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC18" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD18" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE18" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="AF18" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG18" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH18" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="AI18" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="AJ18" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="AK18" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL18" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="AM18" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="AN18" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="AO18" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="AP18" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AQ18" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AR18" s="8"/>
+    </row>
+    <row r="19" spans="1:44" s="19" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="G19" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="H19" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="I19" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="J19" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="K19" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="L19" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="M19" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="N19" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="O19" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="P19" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q19" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="R19" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="S19" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="T19" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="U19" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="V19" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="W19" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="X19" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z19" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="AA19" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="AB19" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="AC19" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="AD19" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="AE19" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="AF19" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="AG19" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="AH19" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="AI19" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="AJ19" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="AK19" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="AL19" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="AM19" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN19" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="AO19" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="AP19" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AQ19" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AR19" s="8"/>
+    </row>
+    <row r="21" spans="1:44" s="23" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="22" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="22" spans="1:44" s="23" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="D22" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="E22" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="F22" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="G22" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="H22" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="I22" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="J22" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="K22" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="L22" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="M22" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="N22" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="O22" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="P22" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q22" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="R22" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="S22" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="T22" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="U22" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="V22" s="23" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="23" spans="1:44" s="23" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="C23" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="E23" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="G23" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="H23" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="I23" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="J23" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="K23" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="L23" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="M23" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="N23" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="O23" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="P23" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q23" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="R23" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="S23" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="T23" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="U23" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="V23" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="AA23" s="22"/>
+      <c r="AG23" s="24"/>
+      <c r="AH23" s="24"/>
+      <c r="AI23" s="25"/>
+      <c r="AL23" s="25"/>
+    </row>
+    <row r="25" spans="1:44" s="27" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="26" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="26" spans="1:44" s="27" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="27" t="s">
+        <v>152</v>
+      </c>
+      <c r="B26" s="27" t="s">
+        <v>153</v>
+      </c>
+      <c r="C26" s="27" t="s">
+        <v>154</v>
+      </c>
+      <c r="D26" s="27" t="s">
+        <v>159</v>
+      </c>
+      <c r="E26" s="27" t="s">
+        <v>160</v>
+      </c>
+      <c r="F26" s="27" t="s">
+        <v>163</v>
+      </c>
+      <c r="G26" s="27" t="s">
+        <v>164</v>
+      </c>
+      <c r="H26" s="27" t="s">
+        <v>167</v>
+      </c>
+      <c r="I26" s="27" t="s">
+        <v>168</v>
+      </c>
+      <c r="J26" s="27" t="s">
+        <v>169</v>
+      </c>
+      <c r="K26" s="27" t="s">
+        <v>171</v>
+      </c>
+      <c r="L26" s="27" t="s">
+        <v>172</v>
+      </c>
+      <c r="M26" s="27" t="s">
+        <v>169</v>
+      </c>
+      <c r="N26" s="27" t="s">
+        <v>243</v>
+      </c>
+      <c r="O26" s="27" t="s">
+        <v>174</v>
+      </c>
+      <c r="P26" s="27" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q26" s="27" t="s">
+        <v>237</v>
+      </c>
+      <c r="R26" s="27" t="s">
+        <v>238</v>
+      </c>
+      <c r="S26" s="27" t="s">
+        <v>242</v>
+      </c>
+      <c r="T26" s="27" t="s">
+        <v>244</v>
+      </c>
+      <c r="U26" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="V26" s="27" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="27" spans="1:44" s="27" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="27" t="s">
+        <v>157</v>
+      </c>
+      <c r="C27" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="D27" s="27" t="s">
+        <v>162</v>
+      </c>
+      <c r="E27" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="F27" s="27" t="s">
+        <v>165</v>
+      </c>
+      <c r="G27" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="H27" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="I27" s="27" t="s">
+        <v>170</v>
+      </c>
+      <c r="J27" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="K27" s="27" t="s">
+        <v>165</v>
+      </c>
+      <c r="L27" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="M27" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="N27" s="28" t="s">
+        <v>241</v>
+      </c>
+      <c r="O27" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="P27" s="28" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q27" s="28" t="s">
+        <v>239</v>
+      </c>
+      <c r="R27" s="28" t="s">
+        <v>240</v>
+      </c>
+      <c r="S27" s="28" t="s">
+        <v>249</v>
+      </c>
+      <c r="T27" s="28" t="s">
+        <v>250</v>
+      </c>
+      <c r="U27" s="28" t="s">
+        <v>247</v>
+      </c>
+      <c r="V27" s="28" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="29" spans="1:44" s="29" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="29" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="30" spans="1:44" s="29" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="29" t="s">
+        <v>194</v>
+      </c>
+      <c r="B30" s="29" t="s">
+        <v>195</v>
+      </c>
+      <c r="C30" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="D30" s="29" t="s">
+        <v>199</v>
+      </c>
+      <c r="E30" s="29" t="s">
+        <v>202</v>
+      </c>
+      <c r="F30" s="29" t="s">
+        <v>204</v>
+      </c>
+      <c r="G30" s="29" t="s">
+        <v>206</v>
+      </c>
+      <c r="H30" s="29" t="s">
+        <v>210</v>
+      </c>
+      <c r="I30" s="29" t="s">
+        <v>209</v>
+      </c>
+      <c r="J30" s="29" t="s">
+        <v>211</v>
+      </c>
+      <c r="K30" s="29" t="s">
+        <v>213</v>
+      </c>
+      <c r="L30" s="29" t="s">
+        <v>214</v>
+      </c>
+      <c r="M30" s="29" t="s">
+        <v>216</v>
+      </c>
+      <c r="N30" s="29" t="s">
+        <v>218</v>
+      </c>
+      <c r="O30" s="29" t="s">
+        <v>220</v>
+      </c>
+      <c r="P30" s="29" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q30" s="29" t="s">
+        <v>224</v>
+      </c>
+      <c r="R30" s="29" t="s">
+        <v>225</v>
+      </c>
+      <c r="S30" s="29" t="s">
+        <v>234</v>
+      </c>
+      <c r="T30" s="29" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="31" spans="1:44" s="29" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="30" t="s">
+        <v>252</v>
+      </c>
+      <c r="B31" s="29" t="s">
+        <v>251</v>
+      </c>
+      <c r="C31" s="29" t="s">
+        <v>253</v>
+      </c>
+      <c r="D31" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="E31" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="F31" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="G31" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="H31" s="30" t="s">
+        <v>208</v>
+      </c>
+      <c r="I31" s="30" t="s">
+        <v>208</v>
+      </c>
+      <c r="J31" s="30" t="s">
+        <v>212</v>
+      </c>
+      <c r="K31" s="29" t="s">
+        <v>227</v>
+      </c>
+      <c r="L31" s="29" t="s">
+        <v>215</v>
+      </c>
+      <c r="M31" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="N31" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="O31" s="29" t="s">
+        <v>219</v>
+      </c>
+      <c r="P31" s="29" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q31" s="29" t="s">
+        <v>223</v>
+      </c>
+      <c r="R31" s="29" t="s">
+        <v>226</v>
+      </c>
+      <c r="S31" s="29" t="s">
+        <v>233</v>
+      </c>
+      <c r="T31" s="29" t="s">
+        <v>255</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="Y3" r:id="rId1" xr:uid="{2F8DBC2D-3C9E-4C2E-89A8-68E0ACD71B93}"/>
+    <hyperlink ref="Y11" r:id="rId2" xr:uid="{3EE8ECB8-9837-4CC6-9076-C1C8D65F5572}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF6A61A0-E1EB-4236-B550-B929F046F19F}">
+  <dimension ref="A1:AR33"/>
+  <sheetViews>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:XFD27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1141,7 +2987,7 @@
     <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.90625" customWidth="1"/>
     <col min="4" max="4" width="11.81640625" customWidth="1"/>
-    <col min="5" max="5" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.26953125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="37.1796875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.453125" customWidth="1"/>
     <col min="8" max="10" width="13.54296875" bestFit="1" customWidth="1"/>
@@ -1167,166 +3013,154 @@
     </row>
     <row r="2" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y2" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>145</v>
+        <v>18</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>146</v>
+        <v>19</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="L3" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="K3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="M3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="O3" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="N3" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="O3" s="23" t="s">
+        <v>228</v>
+      </c>
       <c r="P3" s="2" t="s">
-        <v>153</v>
+        <v>27</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="T3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="U3" s="4" t="s">
+      <c r="S3" s="4" t="s">
         <v>32</v>
       </c>
+      <c r="T3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="V3" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="X3" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="Y3" s="5" t="s">
+      <c r="W3" s="5" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:25" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:25" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
-        <v>1</v>
+        <v>75</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>2</v>
@@ -1362,7 +3196,7 @@
         <v>52</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="N6" s="8" t="s">
         <v>50</v>
@@ -1370,13 +3204,40 @@
       <c r="O6" s="8" t="s">
         <v>51</v>
       </c>
+      <c r="P6" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q6" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="R6" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="S6" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="T6" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="U6" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="V6" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="W6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="X6" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="7" spans="1:25" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="8" t="s">
-        <v>145</v>
+      <c r="A7" s="19" t="s">
+        <v>96</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>8</v>
@@ -1400,16 +3261,16 @@
         <v>14</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L7" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="M7" s="10" t="s">
-        <v>55</v>
+      <c r="M7" s="8" t="s">
+        <v>74</v>
       </c>
       <c r="N7" s="8" t="b">
         <v>1</v>
@@ -1417,10 +3278,37 @@
       <c r="O7" s="8" t="b">
         <v>0</v>
       </c>
+      <c r="P7" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q7" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="R7" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="S7" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="T7" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="U7" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="V7" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="W7" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="X7" s="23" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="9" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G9" s="6"/>
     </row>
@@ -1503,10 +3391,10 @@
     </row>
     <row r="11" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>18</v>
@@ -1547,11 +3435,11 @@
       <c r="O11" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="P11" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q11" s="2" t="s">
-        <v>44</v>
+      <c r="P11" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="Q11" s="23" t="s">
+        <v>228</v>
       </c>
       <c r="R11" s="2" t="s">
         <v>27</v>
@@ -1580,7 +3468,7 @@
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:25" s="8" customFormat="1" x14ac:dyDescent="0.35">
@@ -1591,28 +3479,28 @@
         <v>2</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D14" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F14" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="G14" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="H14" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="I14" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="H14" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="I14" s="8" t="s">
-        <v>82</v>
-      </c>
       <c r="J14" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="K14" s="8" t="s">
         <v>49</v>
@@ -1621,25 +3509,25 @@
         <v>48</v>
       </c>
       <c r="M14" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="N14" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="N14" s="8" t="s">
+      <c r="O14" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="P14" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="O14" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="P14" s="8" t="s">
-        <v>87</v>
-      </c>
       <c r="Q14" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="R14" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="R14" s="8" t="s">
+      <c r="S14" s="8" t="s">
         <v>94</v>
-      </c>
-      <c r="S14" s="8" t="s">
-        <v>96</v>
       </c>
       <c r="T14" s="2" t="s">
         <v>45</v>
@@ -1650,58 +3538,72 @@
     </row>
     <row r="15" spans="1:25" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="E15" s="7"/>
+        <v>96</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="J15" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L15" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="M15" s="10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="N15" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="O15" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="P15" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="P15" s="10" t="s">
+      <c r="Q15" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="Q15" s="8" t="s">
+      <c r="R15" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="R15" s="8" t="s">
+      <c r="S15" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="S15" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="T15" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="U15" s="2" t="s">
-        <v>44</v>
+      <c r="T15" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="U15" s="23" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="17" spans="1:44" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="18" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:44" s="19" customFormat="1" x14ac:dyDescent="0.35">
@@ -1712,64 +3614,64 @@
         <v>2</v>
       </c>
       <c r="C18" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="G18" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="H18" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="I18" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="J18" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="K18" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="L18" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="D18" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="E18" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="F18" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="G18" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="H18" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="I18" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="J18" s="19" t="s">
+      <c r="M18" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="N18" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="K18" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="L18" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="M18" s="19" t="s">
+      <c r="O18" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="N18" s="19" t="s">
+      <c r="P18" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="O18" s="19" t="s">
+      <c r="Q18" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="R18" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="S18" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="P18" s="19" t="s">
+      <c r="T18" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="U18" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="V18" s="19" t="s">
         <v>112</v>
-      </c>
-      <c r="Q18" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="R18" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="S18" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="T18" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="U18" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="V18" s="19" t="s">
-        <v>114</v>
       </c>
       <c r="W18" s="8" t="s">
         <v>1</v>
@@ -1778,28 +3680,28 @@
         <v>2</v>
       </c>
       <c r="Y18" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="Z18" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA18" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB18" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="AA18" s="8" t="s">
+      <c r="AC18" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="AB18" s="8" t="s">
+      <c r="AD18" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="AC18" s="8" t="s">
+      <c r="AE18" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="AD18" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="AE18" s="8" t="s">
-        <v>82</v>
-      </c>
       <c r="AF18" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="AG18" s="8" t="s">
         <v>49</v>
@@ -1808,25 +3710,25 @@
         <v>48</v>
       </c>
       <c r="AI18" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="AJ18" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="AJ18" s="8" t="s">
+      <c r="AK18" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL18" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="AK18" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="AL18" s="8" t="s">
-        <v>87</v>
-      </c>
       <c r="AM18" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="AN18" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="AN18" s="8" t="s">
+      <c r="AO18" s="8" t="s">
         <v>94</v>
-      </c>
-      <c r="AO18" s="8" t="s">
-        <v>96</v>
       </c>
       <c r="AP18" s="2" t="s">
         <v>45</v>
@@ -1838,53 +3740,70 @@
     </row>
     <row r="19" spans="1:44" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="19" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C19" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="G19" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="H19" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="I19" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="J19" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="K19" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="L19" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="M19" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="N19" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="E19" s="18"/>
-      <c r="J19" s="19" t="s">
+      <c r="O19" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="K19" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="L19" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="M19" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="N19" s="19" t="s">
+      <c r="P19" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="O19" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="P19" s="21" t="s">
+      <c r="Q19" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="R19" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="S19" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="T19" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="U19" s="23" t="s">
+        <v>228</v>
+      </c>
+      <c r="V19" s="21" t="s">
         <v>102</v>
-      </c>
-      <c r="Q19" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="R19" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="S19" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="T19" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="U19" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="V19" s="21" t="s">
-        <v>104</v>
       </c>
       <c r="W19" s="8" t="s">
         <v>0</v>
@@ -1893,45 +3812,55 @@
         <v>0</v>
       </c>
       <c r="Y19" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="Z19" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="AA19" s="7"/>
-      <c r="AB19" s="8"/>
-      <c r="AC19" s="8"/>
-      <c r="AD19" s="8"/>
-      <c r="AE19" s="8"/>
+        <v>96</v>
+      </c>
+      <c r="AA19" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="AB19" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="AC19" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="AD19" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="AE19" s="7" t="s">
+        <v>158</v>
+      </c>
       <c r="AF19" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="AG19" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="AH19" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="AI19" s="10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="AJ19" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="AK19" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="AL19" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="AL19" s="10" t="s">
+      <c r="AM19" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="AM19" s="8" t="s">
+      <c r="AN19" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="AN19" s="8" t="s">
+      <c r="AO19" s="8" t="s">
         <v>95</v>
-      </c>
-      <c r="AO19" s="8" t="s">
-        <v>97</v>
       </c>
       <c r="AP19" s="2" t="s">
         <v>43</v>
@@ -1943,7 +3872,7 @@
     </row>
     <row r="21" spans="1:44" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="22" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:44" s="23" customFormat="1" x14ac:dyDescent="0.35">
@@ -1954,115 +3883,132 @@
         <v>2</v>
       </c>
       <c r="C22" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="D22" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="E22" s="23" t="s">
         <v>125</v>
       </c>
-      <c r="D22" s="23" t="s">
+      <c r="F22" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="E22" s="23" t="s">
+      <c r="G22" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="F22" s="23" t="s">
+      <c r="H22" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="G22" s="23" t="s">
+      <c r="I22" s="23" t="s">
         <v>129</v>
       </c>
-      <c r="H22" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="I22" s="23" t="s">
+      <c r="J22" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="J22" s="23" t="s">
+      <c r="K22" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="L22" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="M22" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="K22" s="23" t="s">
-        <v>123</v>
-      </c>
-      <c r="L22" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="M22" s="23" t="s">
+      <c r="N22" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="O22" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="N22" s="23" t="s">
-        <v>136</v>
-      </c>
-      <c r="O22" s="23" t="s">
-        <v>137</v>
-      </c>
       <c r="P22" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q22" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="Q22" s="23" t="s">
-        <v>142</v>
-      </c>
       <c r="R22" s="23" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="S22" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="T22" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="U22" s="23" t="s">
         <v>150</v>
       </c>
-      <c r="T22" s="23" t="s">
-        <v>151</v>
-      </c>
-      <c r="U22" s="23" t="s">
-        <v>152</v>
-      </c>
       <c r="V22" s="23" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="23" spans="1:44" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C23" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="E23" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="G23" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="H23" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="I23" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="J23" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="E23" s="22"/>
-      <c r="J23" s="23" t="s">
-        <v>134</v>
-      </c>
       <c r="K23" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L23" s="24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="M23" s="25" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="N23" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="O23" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="P23" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="O23" s="23" t="s">
-        <v>138</v>
-      </c>
-      <c r="P23" s="25" t="s">
-        <v>141</v>
-      </c>
       <c r="Q23" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="R23" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="R23" s="23" t="s">
+      <c r="S23" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="S23" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="T23" s="23" t="s">
-        <v>43</v>
+      <c r="T23" s="29" t="s">
+        <v>201</v>
       </c>
       <c r="U23" s="23" t="s">
-        <v>44</v>
+        <v>228</v>
       </c>
       <c r="V23" s="25" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AA23" s="22"/>
       <c r="AG23" s="24"/>
@@ -2070,24 +4016,1506 @@
       <c r="AI23" s="25"/>
       <c r="AL23" s="25"/>
     </row>
+    <row r="25" spans="1:44" s="27" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="26" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="26" spans="1:44" s="27" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="27" t="s">
+        <v>152</v>
+      </c>
+      <c r="B26" s="27" t="s">
+        <v>153</v>
+      </c>
+      <c r="C26" s="27" t="s">
+        <v>154</v>
+      </c>
+      <c r="D26" s="27" t="s">
+        <v>159</v>
+      </c>
+      <c r="E26" s="27" t="s">
+        <v>160</v>
+      </c>
+      <c r="F26" s="27" t="s">
+        <v>163</v>
+      </c>
+      <c r="G26" s="27" t="s">
+        <v>164</v>
+      </c>
+      <c r="H26" s="27" t="s">
+        <v>167</v>
+      </c>
+      <c r="I26" s="27" t="s">
+        <v>168</v>
+      </c>
+      <c r="J26" s="27" t="s">
+        <v>169</v>
+      </c>
+      <c r="K26" s="27" t="s">
+        <v>171</v>
+      </c>
+      <c r="L26" s="27" t="s">
+        <v>172</v>
+      </c>
+      <c r="M26" s="27" t="s">
+        <v>169</v>
+      </c>
+      <c r="N26" s="27" t="s">
+        <v>176</v>
+      </c>
+      <c r="O26" s="27" t="s">
+        <v>177</v>
+      </c>
+      <c r="P26" s="27" t="s">
+        <v>178</v>
+      </c>
+      <c r="Q26" s="27" t="s">
+        <v>174</v>
+      </c>
+      <c r="R26" s="27" t="s">
+        <v>175</v>
+      </c>
+      <c r="S26" s="27" t="s">
+        <v>181</v>
+      </c>
+      <c r="T26" s="27" t="s">
+        <v>182</v>
+      </c>
+      <c r="U26" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="V26" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="W26" s="27" t="s">
+        <v>188</v>
+      </c>
+      <c r="X26" s="27" t="s">
+        <v>190</v>
+      </c>
+      <c r="Y26" s="27" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="27" spans="1:44" s="27" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="B27" s="27" t="s">
+        <v>157</v>
+      </c>
+      <c r="C27" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="D27" s="27" t="s">
+        <v>162</v>
+      </c>
+      <c r="E27" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="F27" s="27" t="s">
+        <v>165</v>
+      </c>
+      <c r="G27" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="H27" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="I27" s="27" t="s">
+        <v>170</v>
+      </c>
+      <c r="J27" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="K27" s="27" t="s">
+        <v>165</v>
+      </c>
+      <c r="L27" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="M27" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="N27" s="28" t="s">
+        <v>235</v>
+      </c>
+      <c r="O27" s="28" t="s">
+        <v>179</v>
+      </c>
+      <c r="P27" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="Q27" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="R27" s="28" t="s">
+        <v>235</v>
+      </c>
+      <c r="S27" s="28" t="s">
+        <v>179</v>
+      </c>
+      <c r="T27" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="U27" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="V27" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="W27" s="27" t="s">
+        <v>187</v>
+      </c>
+      <c r="X27" s="28" t="s">
+        <v>235</v>
+      </c>
+      <c r="Y27" s="28" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="30" spans="1:44" s="29" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="29" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="31" spans="1:44" s="29" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="29" t="s">
+        <v>194</v>
+      </c>
+      <c r="B31" s="29" t="s">
+        <v>195</v>
+      </c>
+      <c r="C31" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="D31" s="29" t="s">
+        <v>199</v>
+      </c>
+      <c r="E31" s="29" t="s">
+        <v>202</v>
+      </c>
+      <c r="F31" s="29" t="s">
+        <v>204</v>
+      </c>
+      <c r="G31" s="29" t="s">
+        <v>206</v>
+      </c>
+      <c r="H31" s="29" t="s">
+        <v>210</v>
+      </c>
+      <c r="I31" s="29" t="s">
+        <v>209</v>
+      </c>
+      <c r="J31" s="29" t="s">
+        <v>211</v>
+      </c>
+      <c r="K31" s="29" t="s">
+        <v>213</v>
+      </c>
+      <c r="L31" s="29" t="s">
+        <v>214</v>
+      </c>
+      <c r="M31" s="29" t="s">
+        <v>216</v>
+      </c>
+      <c r="N31" s="29" t="s">
+        <v>218</v>
+      </c>
+      <c r="O31" s="29" t="s">
+        <v>220</v>
+      </c>
+      <c r="P31" s="29" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q31" s="29" t="s">
+        <v>224</v>
+      </c>
+      <c r="R31" s="29" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="32" spans="1:44" s="29" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="29" t="s">
+        <v>193</v>
+      </c>
+      <c r="B32" s="29" t="s">
+        <v>196</v>
+      </c>
+      <c r="C32" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="D32" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="E32" s="29" t="s">
+        <v>203</v>
+      </c>
+      <c r="F32" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="G32" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="H32" s="30" t="s">
+        <v>208</v>
+      </c>
+      <c r="I32" s="30" t="s">
+        <v>208</v>
+      </c>
+      <c r="J32" s="30" t="s">
+        <v>212</v>
+      </c>
+      <c r="K32" s="29" t="s">
+        <v>227</v>
+      </c>
+      <c r="L32" s="29" t="s">
+        <v>215</v>
+      </c>
+      <c r="M32" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="N32" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="O32" s="29" t="s">
+        <v>219</v>
+      </c>
+      <c r="P32" s="29" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q32" s="29" t="s">
+        <v>223</v>
+      </c>
+      <c r="R32" s="29" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A33" s="29" t="s">
+        <v>229</v>
+      </c>
+      <c r="B33" s="29" t="s">
+        <v>230</v>
+      </c>
+      <c r="C33" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="D33" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="E33" s="29" t="s">
+        <v>203</v>
+      </c>
+      <c r="F33" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="G33" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="H33" s="30" t="s">
+        <v>231</v>
+      </c>
+      <c r="I33" s="30" t="s">
+        <v>231</v>
+      </c>
+      <c r="J33" s="30" t="s">
+        <v>212</v>
+      </c>
+      <c r="K33" s="29" t="s">
+        <v>232</v>
+      </c>
+      <c r="L33" s="29" t="s">
+        <v>215</v>
+      </c>
+      <c r="M33" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="N33" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="O33" s="29" t="s">
+        <v>219</v>
+      </c>
+      <c r="P33" s="29" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q33" s="29" t="s">
+        <v>223</v>
+      </c>
+      <c r="R33" s="29" t="s">
+        <v>226</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="Y3" r:id="rId1" xr:uid="{2F8DBC2D-3C9E-4C2E-89A8-68E0ACD71B93}"/>
-    <hyperlink ref="Y11" r:id="rId2" xr:uid="{3EE8ECB8-9837-4CC6-9076-C1C8D65F5572}"/>
+    <hyperlink ref="W3" r:id="rId1" xr:uid="{99500325-F96A-4ACF-BAC6-B234202A8851}"/>
+    <hyperlink ref="Y11" r:id="rId2" xr:uid="{66783667-D183-45C7-ACE1-DBFA29058265}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{579C09BE-0AA8-4E72-B77C-C9E1EC3B70FC}">
+  <dimension ref="A1:AR27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="N9" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="31.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.90625" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" customWidth="1"/>
+    <col min="5" max="5" width="37.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.453125" customWidth="1"/>
+    <col min="8" max="10" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.6328125" customWidth="1"/>
+    <col min="14" max="14" width="26" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="25" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="28.81640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="25.6328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="46.90625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="31.81640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="32.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="6"/>
+    </row>
+    <row r="2" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="V3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="X3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y3" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="N6" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="O6" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="P6" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q6" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="R6" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="S6" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="T6" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="U6" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="V6" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="W6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="X6" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="L7" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="N7" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="O7" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="P7" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q7" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="R7" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="S7" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="T7" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="U7" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="V7" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="W7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="X7" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="U10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="V10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="W10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="X10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y10" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="U11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="V11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="W11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="X11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y11" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A13" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="L14" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="M14" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="N14" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="O14" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="P14" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q14" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="R14" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="S14" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="T14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="U14" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="K15" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="L15" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="M15" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="N15" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="O15" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="P15" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q15" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="R15" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="S15" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="T15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="U15" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:44" s="19" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="18" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:44" s="19" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="G18" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="H18" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="I18" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="J18" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="K18" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="L18" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="M18" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="N18" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="O18" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="P18" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q18" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="R18" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="S18" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="T18" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="U18" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="V18" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="W18" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="X18" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y18" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z18" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA18" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB18" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC18" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD18" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE18" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="AF18" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG18" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH18" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="AI18" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="AJ18" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="AK18" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL18" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="AM18" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="AN18" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="AO18" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="AP18" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AQ18" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AR18" s="8"/>
+    </row>
+    <row r="19" spans="1:44" s="19" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="G19" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="H19" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="I19" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="J19" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="K19" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="L19" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="M19" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="N19" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="O19" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="P19" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q19" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="R19" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="S19" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="T19" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="U19" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="V19" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="W19" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="X19" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z19" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="AA19" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="AB19" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="AC19" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="AD19" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="AE19" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="AF19" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="AG19" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="AH19" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="AI19" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="AJ19" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="AK19" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="AL19" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="AM19" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN19" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="AO19" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="AP19" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AQ19" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AR19" s="8"/>
+    </row>
+    <row r="21" spans="1:44" s="23" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="22" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="22" spans="1:44" s="23" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="D22" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="E22" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="F22" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="G22" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="H22" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="I22" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="J22" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="K22" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="L22" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="M22" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="N22" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="O22" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="P22" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q22" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="R22" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="S22" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="T22" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="U22" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="V22" s="23" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="23" spans="1:44" s="23" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="C23" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="E23" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="G23" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="H23" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="I23" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="J23" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="K23" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="L23" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="M23" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="N23" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="O23" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="P23" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q23" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="R23" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="S23" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="T23" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="U23" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="V23" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="AA23" s="22"/>
+      <c r="AG23" s="24"/>
+      <c r="AH23" s="24"/>
+      <c r="AI23" s="25"/>
+      <c r="AL23" s="25"/>
+    </row>
+    <row r="25" spans="1:44" s="27" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="26" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="26" spans="1:44" s="27" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="27" t="s">
+        <v>152</v>
+      </c>
+      <c r="B26" s="27" t="s">
+        <v>153</v>
+      </c>
+      <c r="C26" s="27" t="s">
+        <v>154</v>
+      </c>
+      <c r="D26" s="27" t="s">
+        <v>159</v>
+      </c>
+      <c r="E26" s="27" t="s">
+        <v>160</v>
+      </c>
+      <c r="F26" s="27" t="s">
+        <v>163</v>
+      </c>
+      <c r="G26" s="27" t="s">
+        <v>164</v>
+      </c>
+      <c r="H26" s="27" t="s">
+        <v>167</v>
+      </c>
+      <c r="I26" s="27" t="s">
+        <v>168</v>
+      </c>
+      <c r="J26" s="27" t="s">
+        <v>169</v>
+      </c>
+      <c r="K26" s="27" t="s">
+        <v>171</v>
+      </c>
+      <c r="L26" s="27" t="s">
+        <v>172</v>
+      </c>
+      <c r="M26" s="27" t="s">
+        <v>169</v>
+      </c>
+      <c r="N26" s="27" t="s">
+        <v>175</v>
+      </c>
+      <c r="O26" s="27" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="27" spans="1:44" s="27" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="27" t="s">
+        <v>157</v>
+      </c>
+      <c r="C27" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="D27" s="27" t="s">
+        <v>162</v>
+      </c>
+      <c r="E27" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="F27" s="27" t="s">
+        <v>165</v>
+      </c>
+      <c r="G27" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="H27" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="I27" s="27" t="s">
+        <v>170</v>
+      </c>
+      <c r="J27" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="K27" s="27" t="s">
+        <v>165</v>
+      </c>
+      <c r="L27" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="M27" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="N27" s="28" t="s">
+        <v>183</v>
+      </c>
+      <c r="O27" s="27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="Y3" r:id="rId1" xr:uid="{7FCA3961-E402-4428-917C-B8DE4265C0F4}"/>
+    <hyperlink ref="Y11" r:id="rId2" xr:uid="{74247AA1-265F-42BD-8019-F76F57528ABA}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
22 december regression test code
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/Test_Data_Sheet.xlsx
+++ b/src/test/resources/testdata/Test_Data_Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sunil\eclipse-workspace\Regression_Pos_project\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B91A4BF2-2AB9-4D90-BFA7-A2560F43A394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E0D1A84-58C2-4E50-B2E5-72345B8F0D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="751" activeTab="5" xr2:uid="{52826312-55BE-45F7-9B29-2F6A9A52A5DF}"/>
+    <workbookView xWindow="20" yWindow="20" windowWidth="19180" windowHeight="10060" tabRatio="751" activeTab="2" xr2:uid="{52826312-55BE-45F7-9B29-2F6A9A52A5DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="2" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3621" uniqueCount="681">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3647" uniqueCount="692">
   <si>
     <t>admin</t>
   </si>
@@ -2406,10 +2406,43 @@
     <t>Active status through Edit Promotion</t>
   </si>
   <si>
-    <t>"Override status through Edit Promotion"</t>
-  </si>
-  <si>
     <t xml:space="preserve">Smoke </t>
+  </si>
+  <si>
+    <t>Override status through Edit Promotion</t>
+  </si>
+  <si>
+    <t>Store Selection for Edit store</t>
+  </si>
+  <si>
+    <t>MasterPromotion_TestCases</t>
+  </si>
+  <si>
+    <t>Metawear Limited Kolkata - 1001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Master Promotion Screen Test Case </t>
+  </si>
+  <si>
+    <t>edit_Promotion_from_Promotion_Table</t>
+  </si>
+  <si>
+    <t>Master-001</t>
+  </si>
+  <si>
+    <t>This test case will cover all the operations related to edit promotion . It will also display all the skus in the report which has uploaded through edit . You can cross check with your product file .</t>
+  </si>
+  <si>
+    <t>Store Selection for Edit store,Override status through Edit Promotion,Active status through Edit Promotion,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">File Name to Upload </t>
+  </si>
+  <si>
+    <t>Promoset1,Promoset2</t>
+  </si>
+  <si>
+    <t>Store Selection for Edit store all type of promotion apart from combination pool</t>
   </si>
 </sst>
 </file>
@@ -2419,7 +2452,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2501,6 +2534,12 @@
     <font>
       <sz val="10"/>
       <color rgb="FF118BBD"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF1DAF3E"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
@@ -2850,7 +2889,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -3115,6 +3154,7 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3468,23 +3508,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="8"/>
+    <col min="1" max="1" width="8.7265625" style="8"/>
     <col min="2" max="2" width="43" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" style="10"/>
-    <col min="4" max="4" width="11.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7109375" style="13"/>
+    <col min="3" max="3" width="8.7265625" style="10"/>
+    <col min="4" max="4" width="11.54296875" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.54296875" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.7265625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>57</v>
       </c>
@@ -3501,24 +3541,24 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
-        <v>594</v>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B2" s="70" t="s">
+        <v>682</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="70" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B3" s="9" t="s">
         <v>458</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="117"/>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B5" s="117"/>
     </row>
   </sheetData>
   <autoFilter ref="C1" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
@@ -3542,14 +3582,14 @@
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="37.453125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="35.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" s="13" customFormat="1" ht="16" x14ac:dyDescent="0.4">
       <c r="A1" s="8">
         <v>1</v>
       </c>
@@ -3565,29 +3605,29 @@
       <c r="E1" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="I1" s="118" t="s">
+      <c r="I1" s="119" t="s">
         <v>497</v>
       </c>
-      <c r="J1" s="119"/>
-      <c r="K1" s="119"/>
-      <c r="L1" s="119"/>
-      <c r="M1" s="120"/>
-      <c r="O1" s="121" t="s">
+      <c r="J1" s="120"/>
+      <c r="K1" s="120"/>
+      <c r="L1" s="120"/>
+      <c r="M1" s="121"/>
+      <c r="O1" s="122" t="s">
         <v>498</v>
       </c>
-      <c r="P1" s="122"/>
-      <c r="Q1" s="122"/>
-      <c r="R1" s="122"/>
-      <c r="S1" s="123"/>
-      <c r="V1" s="118" t="s">
+      <c r="P1" s="123"/>
+      <c r="Q1" s="123"/>
+      <c r="R1" s="123"/>
+      <c r="S1" s="124"/>
+      <c r="V1" s="119" t="s">
         <v>501</v>
       </c>
-      <c r="W1" s="119"/>
-      <c r="X1" s="119"/>
-      <c r="Y1" s="119"/>
-      <c r="Z1" s="120"/>
-    </row>
-    <row r="2" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="W1" s="120"/>
+      <c r="X1" s="120"/>
+      <c r="Y1" s="120"/>
+      <c r="Z1" s="121"/>
+    </row>
+    <row r="2" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8">
         <v>2</v>
       </c>
@@ -3649,7 +3689,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8">
         <v>3</v>
       </c>
@@ -3701,7 +3741,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="8">
         <v>4</v>
       </c>
@@ -3753,7 +3793,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="8">
         <v>5</v>
       </c>
@@ -3777,7 +3817,7 @@
         <v>67</v>
       </c>
       <c r="L5" s="11" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="M5" s="12"/>
       <c r="O5" s="8"/>
@@ -3805,7 +3845,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="8">
         <v>6</v>
       </c>
@@ -3842,7 +3882,7 @@
       <c r="R6" s="11"/>
       <c r="S6" s="12"/>
     </row>
-    <row r="7" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="8">
         <v>7</v>
       </c>
@@ -3866,7 +3906,7 @@
         <v>67</v>
       </c>
       <c r="L7" s="11" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="M7" s="12"/>
       <c r="O7" s="8"/>
@@ -3875,7 +3915,7 @@
       <c r="R7" s="11"/>
       <c r="S7" s="12"/>
     </row>
-    <row r="8" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="8">
         <v>8</v>
       </c>
@@ -3908,7 +3948,7 @@
       <c r="R8"/>
       <c r="S8"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A9" s="83">
         <v>9</v>
       </c>
@@ -3936,7 +3976,7 @@
       </c>
       <c r="M9" s="12"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A10" s="83">
         <v>10</v>
       </c>
@@ -3964,7 +4004,7 @@
       </c>
       <c r="M10" s="12"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A11" s="83">
         <v>11</v>
       </c>
@@ -3991,7 +4031,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B12" s="6" t="s">
         <v>462</v>
       </c>
@@ -4003,7 +4043,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
       <c r="Q13" s="8">
         <v>1</v>
       </c>
@@ -4020,7 +4060,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
       <c r="Q14" s="8">
         <v>2</v>
       </c>
@@ -4033,7 +4073,7 @@
       <c r="T14" s="11"/>
       <c r="U14" s="12"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
       <c r="T15" s="11" t="s">
         <v>61</v>
       </c>
@@ -4041,7 +4081,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
       <c r="T16" s="11" t="s">
         <v>61</v>
       </c>
@@ -4069,232 +4109,220 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:AD24"/>
+  <dimension ref="A2:AD28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="48.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="46.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="41.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="44.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="42.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="45.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="40.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="45.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="49.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="46.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="43.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="44.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="45.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="48.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="46.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="41.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="44.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="42.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="45.453125" style="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="39.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="40.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="45.81640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="49.81640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="46.54296875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="43.81640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="28.81640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="44.7265625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="45.81640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="35.453125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="42" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="44.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="42.42578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="29" width="41.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="32" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="44.26953125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="42.453125" bestFit="1" customWidth="1"/>
+    <col min="27" max="29" width="41.81640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="32" width="38.1796875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="30.453125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="29.453125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="28.81640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="25.54296875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="25.81640625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="11.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="70" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="3" spans="1:30" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="69" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="B3" s="69" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="C3" s="69" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="D3" s="69" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="E3" s="69" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
       <c r="F3" s="69" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="G3" s="69" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="H3" s="69" t="s">
-        <v>669</v>
+        <v>99</v>
       </c>
       <c r="I3" s="69" t="s">
-        <v>668</v>
+        <v>103</v>
       </c>
       <c r="J3" s="69" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="K3" s="69" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="L3" s="69" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M3" s="69" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="N3" s="69" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="O3" s="69" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="P3" s="69" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="Q3" s="69" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="R3" s="69" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="S3" s="69" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="T3" s="69" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="U3" s="69" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="V3" s="69" t="s">
-        <v>109</v>
+        <v>75</v>
       </c>
       <c r="W3" s="69" t="s">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="X3" s="69" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="Y3" s="69" t="s">
-        <v>84</v>
-      </c>
-      <c r="Z3" s="69" t="s">
-        <v>77</v>
-      </c>
-      <c r="AA3" s="69" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:30" s="69" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="69" t="b">
-        <v>1</v>
-      </c>
-      <c r="B4" s="74" t="b">
-        <v>0</v>
+    <row r="4" spans="1:30" s="69" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="69" t="s">
+        <v>675</v>
+      </c>
+      <c r="B4" s="69" t="s">
+        <v>677</v>
       </c>
       <c r="C4" s="69" t="s">
-        <v>675</v>
+        <v>540</v>
       </c>
       <c r="D4" s="69" t="s">
-        <v>677</v>
+        <v>537</v>
       </c>
       <c r="E4" s="69" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="F4" s="69" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G4" s="69" t="s">
-        <v>542</v>
+        <v>89</v>
       </c>
       <c r="H4" s="69" t="s">
-        <v>536</v>
-      </c>
-      <c r="I4" s="69" t="s">
+        <v>92</v>
+      </c>
+      <c r="I4" s="74" t="s">
+        <v>78</v>
+      </c>
+      <c r="J4" s="69" t="s">
+        <v>460</v>
+      </c>
+      <c r="K4" s="75" t="s">
+        <v>413</v>
+      </c>
+      <c r="L4" s="75" t="s">
+        <v>416</v>
+      </c>
+      <c r="M4" s="69" t="s">
+        <v>94</v>
+      </c>
+      <c r="N4" s="69" t="s">
+        <v>95</v>
+      </c>
+      <c r="O4" s="74" t="s">
+        <v>96</v>
+      </c>
+      <c r="P4" s="69" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q4" s="69" t="s">
         <v>89</v>
       </c>
-      <c r="J4" s="69" t="s">
+      <c r="R4" s="69" t="s">
+        <v>91</v>
+      </c>
+      <c r="S4" s="69" t="s">
+        <v>43</v>
+      </c>
+      <c r="T4" s="69" t="s">
+        <v>44</v>
+      </c>
+      <c r="U4" s="74" t="s">
+        <v>98</v>
+      </c>
+      <c r="V4" s="69" t="s">
         <v>92</v>
       </c>
-      <c r="K4" s="74" t="s">
+      <c r="W4" s="69" t="s">
+        <v>74</v>
+      </c>
+      <c r="X4" s="74" t="s">
         <v>78</v>
       </c>
-      <c r="L4" s="69" t="s">
-        <v>460</v>
-      </c>
-      <c r="M4" s="75" t="s">
-        <v>413</v>
-      </c>
-      <c r="N4" s="75" t="s">
-        <v>416</v>
-      </c>
-      <c r="O4" s="69" t="s">
-        <v>94</v>
-      </c>
-      <c r="P4" s="69" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q4" s="74" t="s">
-        <v>96</v>
-      </c>
-      <c r="R4" s="69" t="s">
+      <c r="Y4" s="69" t="s">
         <v>87</v>
       </c>
-      <c r="S4" s="69" t="s">
-        <v>89</v>
-      </c>
-      <c r="T4" s="69" t="s">
-        <v>91</v>
-      </c>
-      <c r="U4" s="69" t="s">
-        <v>43</v>
-      </c>
-      <c r="V4" s="69" t="s">
-        <v>44</v>
-      </c>
-      <c r="W4" s="74" t="s">
-        <v>98</v>
-      </c>
-      <c r="X4" s="69" t="s">
-        <v>92</v>
-      </c>
-      <c r="Y4" s="69" t="s">
-        <v>74</v>
-      </c>
-      <c r="Z4" s="74" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA4" s="69" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="6" spans="1:30" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:30" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="7" spans="1:30" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="69" t="s">
         <v>115</v>
       </c>
@@ -4338,7 +4366,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="8" spans="1:30" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="69" t="s">
         <v>122</v>
       </c>
@@ -4387,12 +4415,12 @@
       <c r="AA8" s="74"/>
       <c r="AD8" s="74"/>
     </row>
-    <row r="10" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="11" spans="1:30" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="69" t="s">
         <v>115</v>
       </c>
@@ -4436,7 +4464,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="12" spans="1:30" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="69" t="s">
         <v>122</v>
       </c>
@@ -4485,13 +4513,13 @@
       <c r="AA12" s="74"/>
       <c r="AD12" s="74"/>
     </row>
-    <row r="14" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="49" t="s">
         <v>513</v>
       </c>
       <c r="M14" s="86"/>
     </row>
-    <row r="15" spans="1:30" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="69" t="s">
         <v>49</v>
       </c>
@@ -4571,7 +4599,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:30" s="29" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" s="29" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="75" t="s">
         <v>70</v>
       </c>
@@ -4651,13 +4679,13 @@
         <v>541</v>
       </c>
     </row>
-    <row r="18" spans="1:28" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="49" t="s">
         <v>543</v>
       </c>
       <c r="M18" s="86"/>
     </row>
-    <row r="19" spans="1:28" s="29" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" s="29" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="69" t="s">
         <v>49</v>
       </c>
@@ -4743,7 +4771,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="20" spans="1:28" s="29" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" s="29" customFormat="1" ht="32.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="75" t="s">
         <v>70</v>
       </c>
@@ -4829,13 +4857,13 @@
         <v>544</v>
       </c>
     </row>
-    <row r="22" spans="1:28" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="70" t="s">
         <v>594</v>
       </c>
       <c r="M22" s="86"/>
     </row>
-    <row r="23" spans="1:28" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="69" t="s">
         <v>657</v>
       </c>
@@ -4880,7 +4908,7 @@
       </c>
       <c r="R23" s="33"/>
     </row>
-    <row r="24" spans="1:28" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="74" t="s">
         <v>658</v>
       </c>
@@ -4924,6 +4952,68 @@
         <v>98</v>
       </c>
       <c r="R24" s="33"/>
+    </row>
+    <row r="26" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="7" t="s">
+        <v>682</v>
+      </c>
+      <c r="M26" s="92"/>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>691</v>
+      </c>
+      <c r="B27" s="69" t="s">
+        <v>681</v>
+      </c>
+      <c r="C27" s="69" t="s">
+        <v>680</v>
+      </c>
+      <c r="D27" s="69" t="s">
+        <v>678</v>
+      </c>
+      <c r="E27" s="69" t="s">
+        <v>49</v>
+      </c>
+      <c r="F27" s="69" t="s">
+        <v>48</v>
+      </c>
+      <c r="G27" s="69" t="s">
+        <v>50</v>
+      </c>
+      <c r="H27" s="69" t="s">
+        <v>51</v>
+      </c>
+      <c r="M27"/>
+      <c r="N27" s="17"/>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A28" s="69" t="s">
+        <v>683</v>
+      </c>
+      <c r="B28" s="69" t="s">
+        <v>683</v>
+      </c>
+      <c r="C28" s="69" t="b">
+        <v>1</v>
+      </c>
+      <c r="D28" s="69" t="b">
+        <v>1</v>
+      </c>
+      <c r="E28" s="75" t="s">
+        <v>70</v>
+      </c>
+      <c r="F28" s="75" t="s">
+        <v>71</v>
+      </c>
+      <c r="G28" s="69" t="b">
+        <v>1</v>
+      </c>
+      <c r="H28" s="69" t="b">
+        <v>0</v>
+      </c>
+      <c r="M28"/>
+      <c r="N28" s="17"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -4939,41 +5029,41 @@
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35.42578125" style="29" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.453125" style="29" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" style="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.28515625" style="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.5703125" style="29" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.5703125" style="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" style="29" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" style="29" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.85546875" style="29" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.7109375" style="29" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.28515625" style="29" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="36.140625" style="29" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="40.7109375" style="29" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="30.5703125" style="29" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="39.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="40.85546875" style="29" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="39.140625" style="29" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="49.85546875" style="29" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="46.5703125" style="29" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="43.85546875" style="29" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.85546875" style="29" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="44.7109375" style="29" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="53.5703125" style="29" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="35.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="33.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="25" max="16384" width="8.7109375" style="29"/>
+    <col min="3" max="3" width="41.26953125" style="29" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.54296875" style="29" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.54296875" style="29" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.1796875" style="29" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.81640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.81640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.7265625" style="29" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.26953125" style="29" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="36.1796875" style="29" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="40.7265625" style="29" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="30.54296875" style="29" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="39.453125" style="29" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="40.81640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="39.1796875" style="29" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="49.81640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="46.54296875" style="29" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="43.81640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.81640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="44.7265625" style="29" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="53.54296875" style="29" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="35.453125" style="29" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="33.453125" style="29" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="8.7265625" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="26" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" s="26" customFormat="1" ht="23.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="25" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:31" s="26" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" s="26" customFormat="1" ht="23.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="26" t="s">
         <v>174</v>
       </c>
@@ -5047,7 +5137,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="3" spans="1:31" s="26" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" s="26" customFormat="1" ht="23.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="27"/>
       <c r="H3" s="27"/>
       <c r="I3" s="27"/>
@@ -5083,12 +5173,12 @@
         <v>250</v>
       </c>
     </row>
-    <row r="5" spans="1:31" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="25" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="6" spans="1:31" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="26" t="s">
         <v>174</v>
       </c>
@@ -5162,7 +5252,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="7" spans="1:31" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="27"/>
       <c r="H7" s="27"/>
       <c r="I7" s="27"/>
@@ -5198,12 +5288,12 @@
         <v>250</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A9" s="25" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="10" spans="1:31" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="26" t="s">
         <v>142</v>
       </c>
@@ -5253,7 +5343,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="11" spans="1:31" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C11" s="27"/>
       <c r="D11" s="27"/>
       <c r="E11" s="26" t="s">
@@ -5269,12 +5359,12 @@
       <c r="U11" s="27"/>
       <c r="V11" s="27"/>
     </row>
-    <row r="13" spans="1:31" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="70" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="14" spans="1:31" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="69" t="s">
         <v>99</v>
       </c>
@@ -5369,7 +5459,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:31" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="69" t="s">
         <v>92</v>
       </c>
@@ -5464,12 +5554,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:14" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="70" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:14" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="69" t="s">
         <v>72</v>
       </c>
@@ -5513,7 +5603,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:14" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="69" t="s">
         <v>73</v>
       </c>
@@ -5557,7 +5647,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:14" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="69" t="s">
         <v>73</v>
       </c>
@@ -5601,7 +5691,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:14" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="69" t="s">
         <v>73</v>
       </c>
@@ -5654,59 +5744,59 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF6A61A0-E1EB-4236-B550-B929F046F19F}">
   <dimension ref="A1:AL80"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45:XFD45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" style="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.28515625" style="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.140625" style="29" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.28515625" style="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="48.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="46.5703125" style="29" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.85546875" style="29" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.453125" style="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.54296875" style="29" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.26953125" style="29" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.1796875" style="29" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.26953125" style="29" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="48.453125" style="29" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="46.54296875" style="29" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.81640625" style="29" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="31" style="29" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.140625" style="29" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="44.28515625" style="29" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="42.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="45.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="39.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="40.85546875" style="29" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="39.140625" style="29" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="49.85546875" style="29" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="46.5703125" style="29" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="43.85546875" style="29" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.1796875" style="29" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="44.26953125" style="29" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="42.453125" style="29" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="45.453125" style="29" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="39.453125" style="29" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="40.81640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="39.1796875" style="29" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="49.81640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="46.54296875" style="29" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="43.81640625" style="29" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="32" style="29" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="44.7109375" style="29" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="46.140625" style="29" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="35.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="44.28515625" style="29" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="44.7265625" style="29" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="46.1796875" style="29" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="35.453125" style="29" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="44.26953125" style="29" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="42" style="29" bestFit="1" customWidth="1"/>
-    <col min="27" max="32" width="14.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="30.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="29.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="17.5703125" style="29" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="13.85546875" style="29" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="18.85546875" style="29" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="13.140625" style="29" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="28.85546875" style="29" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="25.5703125" style="29" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="11.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="25.85546875" style="29" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="11.5703125" style="29" bestFit="1" customWidth="1"/>
-    <col min="44" max="16384" width="8.7109375" style="29"/>
+    <col min="27" max="32" width="14.453125" style="29" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="30.453125" style="29" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="29.453125" style="29" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="17.54296875" style="29" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.81640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="18.81640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="13.1796875" style="29" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="28.81640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="25.54296875" style="29" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11.453125" style="29" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="25.81640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="11.54296875" style="29" bestFit="1" customWidth="1"/>
+    <col min="44" max="16384" width="8.7265625" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="63" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="63"/>
     </row>
-    <row r="2" spans="1:26" s="64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" s="64" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="64" t="s">
         <v>16</v>
       </c>
@@ -5777,7 +5867,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" s="64" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="64" t="s">
         <v>18</v>
       </c>
@@ -5848,12 +5938,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:26" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="63" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:26" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="49" t="s">
         <v>72</v>
       </c>
@@ -5933,7 +6023,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="7" spans="1:26" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="49" t="s">
         <v>73</v>
       </c>
@@ -6013,13 +6103,13 @@
         <v>179</v>
       </c>
     </row>
-    <row r="9" spans="1:26" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="63" t="s">
         <v>66</v>
       </c>
       <c r="G9" s="63"/>
     </row>
-    <row r="10" spans="1:26" s="64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" s="64" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="64" t="s">
         <v>1</v>
       </c>
@@ -6096,7 +6186,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:26" s="64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" s="64" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="64" t="s">
         <v>135</v>
       </c>
@@ -6173,12 +6263,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:26" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="63" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:26" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="49" t="s">
         <v>72</v>
       </c>
@@ -6222,7 +6312,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:26" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="49" t="s">
         <v>73</v>
       </c>
@@ -6266,12 +6356,12 @@
         <v>205</v>
       </c>
     </row>
-    <row r="18" spans="1:38" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:38" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="63" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="19" spans="1:38" s="64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:38" s="64" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="64" t="s">
         <v>1</v>
       </c>
@@ -6339,7 +6429,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="20" spans="1:38" s="64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:38" s="64" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="64" t="s">
         <v>135</v>
       </c>
@@ -6412,12 +6502,12 @@
       <c r="AI20" s="67"/>
       <c r="AL20" s="67"/>
     </row>
-    <row r="22" spans="1:38" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:38" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="63" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="23" spans="1:38" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:38" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
         <v>142</v>
       </c>
@@ -6500,7 +6590,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="24" spans="1:38" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:38" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="49" t="s">
         <v>551</v>
       </c>
@@ -6583,12 +6673,12 @@
         <v>209</v>
       </c>
     </row>
-    <row r="26" spans="1:38" s="73" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:38" s="73" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="73" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="27" spans="1:38" s="64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:38" s="64" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="64" t="s">
         <v>174</v>
       </c>
@@ -6686,7 +6776,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="28" spans="1:38" s="64" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:38" s="64" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="67" t="s">
         <v>231</v>
       </c>
@@ -6760,12 +6850,12 @@
         <v>369</v>
       </c>
     </row>
-    <row r="30" spans="1:38" s="73" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:38" s="73" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="73" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="31" spans="1:38" s="64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:38" s="64" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="64" t="s">
         <v>174</v>
       </c>
@@ -6872,7 +6962,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="32" spans="1:38" s="64" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:38" s="64" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="67" t="s">
         <v>278</v>
       </c>
@@ -6955,12 +7045,12 @@
         <v>383</v>
       </c>
     </row>
-    <row r="34" spans="1:22" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:22" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="11" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="35" spans="1:22" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:22" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="49" t="s">
         <v>72</v>
       </c>
@@ -7004,7 +7094,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:22" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:22" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="49" t="s">
         <v>73</v>
       </c>
@@ -7048,12 +7138,12 @@
         <v>205</v>
       </c>
     </row>
-    <row r="38" spans="1:22" s="73" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:22" s="73" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="82" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="39" spans="1:22" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:22" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="49" t="s">
         <v>99</v>
       </c>
@@ -7097,7 +7187,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="40" spans="1:22" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:22" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="49" t="s">
         <v>92</v>
       </c>
@@ -7141,7 +7231,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="41" spans="1:22" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:22" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="49" t="s">
         <v>92</v>
       </c>
@@ -7185,7 +7275,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="42" spans="1:22" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:22" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="49" t="s">
         <v>92</v>
       </c>
@@ -7229,12 +7319,12 @@
         <v>98</v>
       </c>
     </row>
-    <row r="44" spans="1:22" s="73" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:22" s="73" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A44" s="82" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="45" spans="1:22" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:22" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A45" s="49" t="s">
         <v>676</v>
       </c>
@@ -7302,7 +7392,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="46" spans="1:22" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:22" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A46" s="49" t="s">
         <v>675</v>
       </c>
@@ -7370,12 +7460,12 @@
         <v>87</v>
       </c>
     </row>
-    <row r="48" spans="1:22" s="73" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:22" s="73" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A48" s="15" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="49" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="49" t="s">
         <v>115</v>
       </c>
@@ -7419,7 +7509,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="50" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="49" t="s">
         <v>122</v>
       </c>
@@ -7468,12 +7558,12 @@
       <c r="AA50" s="72"/>
       <c r="AD50" s="72"/>
     </row>
-    <row r="53" spans="1:30" s="73" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:30" s="73" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A53" s="15" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="54" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A54" s="49" t="s">
         <v>115</v>
       </c>
@@ -7517,7 +7607,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="55" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A55" s="49" t="s">
         <v>122</v>
       </c>
@@ -7566,13 +7656,13 @@
       <c r="AA55" s="72"/>
       <c r="AD55" s="72"/>
     </row>
-    <row r="57" spans="1:30" s="73" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:30" s="73" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A57" s="73" t="s">
         <v>513</v>
       </c>
       <c r="M57" s="94"/>
     </row>
-    <row r="58" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A58" s="49" t="s">
         <v>49</v>
       </c>
@@ -7655,7 +7745,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="59" spans="1:30" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:30" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="71" t="s">
         <v>70</v>
       </c>
@@ -7738,13 +7828,13 @@
         <v>541</v>
       </c>
     </row>
-    <row r="61" spans="1:30" s="73" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:30" s="73" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A61" s="73" t="s">
         <v>518</v>
       </c>
       <c r="M61" s="94"/>
     </row>
-    <row r="62" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A62" s="49" t="s">
         <v>49</v>
       </c>
@@ -7791,7 +7881,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="63" spans="1:30" s="49" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:30" s="49" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="71" t="s">
         <v>70</v>
       </c>
@@ -7838,13 +7928,13 @@
         <v>44</v>
       </c>
     </row>
-    <row r="65" spans="1:18" s="73" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:18" s="73" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A65" s="82" t="s">
         <v>549</v>
       </c>
       <c r="M65" s="94"/>
     </row>
-    <row r="66" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A66" s="49" t="s">
         <v>643</v>
       </c>
@@ -7892,7 +7982,7 @@
       </c>
       <c r="Q66" s="86"/>
     </row>
-    <row r="67" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A67" s="72" t="s">
         <v>644</v>
       </c>
@@ -7940,13 +8030,13 @@
       </c>
       <c r="Q67" s="86"/>
     </row>
-    <row r="70" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A70" s="15" t="s">
         <v>581</v>
       </c>
       <c r="M70" s="97"/>
     </row>
-    <row r="71" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A71" s="7" t="s">
         <v>582</v>
       </c>
@@ -7976,7 +8066,7 @@
       </c>
       <c r="M71" s="92"/>
     </row>
-    <row r="72" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A72" s="98" t="s">
         <v>585</v>
       </c>
@@ -8006,13 +8096,13 @@
       </c>
       <c r="M72" s="92"/>
     </row>
-    <row r="74" spans="1:18" s="73" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:18" s="73" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A74" s="82" t="s">
         <v>594</v>
       </c>
       <c r="M74" s="94"/>
     </row>
-    <row r="75" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A75" s="49" t="s">
         <v>657</v>
       </c>
@@ -8057,7 +8147,7 @@
       </c>
       <c r="R75" s="86"/>
     </row>
-    <row r="76" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A76" s="72" t="s">
         <v>658</v>
       </c>
@@ -8102,13 +8192,13 @@
       </c>
       <c r="R76" s="86"/>
     </row>
-    <row r="78" spans="1:18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>665</v>
       </c>
       <c r="M78" s="17"/>
     </row>
-    <row r="79" spans="1:18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A79" s="49" t="s">
         <v>657</v>
       </c>
@@ -8117,7 +8207,7 @@
       </c>
       <c r="M79" s="17"/>
     </row>
-    <row r="80" spans="1:18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A80" s="72" t="s">
         <v>667</v>
       </c>
@@ -8140,60 +8230,60 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{579C09BE-0AA8-4E72-B77C-C9E1EC3B70FC}">
   <dimension ref="A1:AL103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="A96" sqref="A96:XFD98"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6:O7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.28515625" style="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.140625" style="29" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.28515625" style="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="48.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="46.5703125" style="29" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.85546875" style="29" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="41.28515625" style="29" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.140625" style="29" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="44.28515625" style="29" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="42.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="45.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="39.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="40.85546875" style="29" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="45.85546875" style="29" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="49.85546875" style="29" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="46.5703125" style="29" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="43.85546875" style="29" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="28.85546875" style="29" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="44.7109375" style="29" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="46.140625" style="29" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="35.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="33.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="41.5703125" style="29" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.453125" style="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.453125" style="29" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.26953125" style="29" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.1796875" style="29" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.26953125" style="29" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="48.453125" style="29" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="46.54296875" style="29" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.81640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="41.26953125" style="29" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.1796875" style="29" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="44.26953125" style="29" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="42.453125" style="29" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="45.453125" style="29" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="39.453125" style="29" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="40.81640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="45.81640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="49.81640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="46.54296875" style="29" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="43.81640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="28.81640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="44.7265625" style="29" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="46.1796875" style="29" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="35.453125" style="29" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="33.453125" style="29" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="41.54296875" style="29" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="42" style="29" bestFit="1" customWidth="1"/>
-    <col min="27" max="32" width="14.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="30.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="29.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="17.5703125" style="29" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="13.85546875" style="29" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="18.85546875" style="29" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="13.140625" style="29" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="28.85546875" style="29" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="25.5703125" style="29" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="11.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="25.85546875" style="29" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="11.5703125" style="29" bestFit="1" customWidth="1"/>
-    <col min="44" max="16384" width="8.7109375" style="29"/>
+    <col min="27" max="32" width="14.453125" style="29" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="30.453125" style="29" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="29.453125" style="29" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="17.54296875" style="29" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.81640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="18.81640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="13.1796875" style="29" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="28.81640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="25.54296875" style="29" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11.453125" style="29" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="25.81640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="11.54296875" style="29" bestFit="1" customWidth="1"/>
+    <col min="44" max="16384" width="8.7265625" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="70" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="70"/>
     </row>
-    <row r="2" spans="1:26" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="69" t="s">
         <v>2</v>
       </c>
@@ -8267,7 +8357,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="69" t="s">
         <v>136</v>
       </c>
@@ -8341,12 +8431,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:26" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="70" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:26" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="69" t="s">
         <v>72</v>
       </c>
@@ -8426,7 +8516,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="7" spans="1:26" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="69" t="s">
         <v>73</v>
       </c>
@@ -8506,13 +8596,13 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:26" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="70" t="s">
         <v>66</v>
       </c>
       <c r="G9" s="70"/>
     </row>
-    <row r="10" spans="1:26" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="69" t="s">
         <v>1</v>
       </c>
@@ -8589,7 +8679,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:26" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="69" t="s">
         <v>135</v>
       </c>
@@ -8666,12 +8756,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:26" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="70" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:26" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="69" t="s">
         <v>72</v>
       </c>
@@ -8715,7 +8805,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:26" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="69" t="s">
         <v>73</v>
       </c>
@@ -8759,7 +8849,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:26" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="69" t="s">
         <v>73</v>
       </c>
@@ -8803,7 +8893,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:38" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:38" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="69" t="s">
         <v>73</v>
       </c>
@@ -8847,19 +8937,19 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:38" x14ac:dyDescent="0.35">
       <c r="B18" s="78"/>
       <c r="D18" s="79"/>
       <c r="E18" s="79"/>
       <c r="F18" s="78"/>
       <c r="I18" s="78"/>
     </row>
-    <row r="20" spans="1:38" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:38" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="70" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="21" spans="1:38" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:38" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="69" t="s">
         <v>1</v>
       </c>
@@ -8927,7 +9017,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="22" spans="1:38" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:38" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="69" t="s">
         <v>135</v>
       </c>
@@ -9000,13 +9090,13 @@
       <c r="AI22" s="74"/>
       <c r="AL22" s="74"/>
     </row>
-    <row r="24" spans="1:38" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:38" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="6" t="s">
         <v>145</v>
       </c>
       <c r="M24" s="92"/>
     </row>
-    <row r="25" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>142</v>
       </c>
@@ -9089,7 +9179,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="26" spans="1:38" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>43</v>
       </c>
@@ -9172,12 +9262,12 @@
         <v>548</v>
       </c>
     </row>
-    <row r="28" spans="1:38" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:38" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="49" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="29" spans="1:38" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:38" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="69" t="s">
         <v>174</v>
       </c>
@@ -9276,7 +9366,7 @@
       </c>
       <c r="AG29" s="26"/>
     </row>
-    <row r="30" spans="1:38" s="69" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:38" s="69" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="74" t="s">
         <v>370</v>
       </c>
@@ -9359,12 +9449,12 @@
       <c r="AF30" s="26"/>
       <c r="AG30" s="26"/>
     </row>
-    <row r="32" spans="1:38" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:38" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="49" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="33" spans="1:35" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:35" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="69" t="s">
         <v>142</v>
       </c>
@@ -9414,7 +9504,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="34" spans="1:35" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:35" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="69" t="s">
         <v>43</v>
       </c>
@@ -9470,12 +9560,12 @@
       <c r="U34" s="74"/>
       <c r="V34" s="74"/>
     </row>
-    <row r="36" spans="1:35" s="64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:35" s="64" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="64" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="37" spans="1:35" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:35" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="69" t="s">
         <v>174</v>
       </c>
@@ -9582,7 +9672,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="38" spans="1:35" s="69" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:35" s="69" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" s="74" t="s">
         <v>373</v>
       </c>
@@ -9689,12 +9779,12 @@
         <v>383</v>
       </c>
     </row>
-    <row r="40" spans="1:35" s="64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:35" s="64" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="64" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="41" spans="1:35" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:35" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="69" t="s">
         <v>174</v>
       </c>
@@ -9801,7 +9891,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="42" spans="1:35" s="69" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:35" s="69" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" s="74" t="s">
         <v>373</v>
       </c>
@@ -9896,12 +9986,12 @@
         <v>383</v>
       </c>
     </row>
-    <row r="44" spans="1:35" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:35" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A44" s="81" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="45" spans="1:35" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:35" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A45" s="69" t="s">
         <v>72</v>
       </c>
@@ -9945,7 +10035,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="46" spans="1:35" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:35" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A46" s="69" t="s">
         <v>73</v>
       </c>
@@ -9989,12 +10079,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="1:35" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:35" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A48" s="70" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="49" spans="1:30" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:30" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="69" t="s">
         <v>99</v>
       </c>
@@ -10038,7 +10128,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="50" spans="1:30" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:30" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="69" t="s">
         <v>92</v>
       </c>
@@ -10082,7 +10172,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="51" spans="1:30" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:30" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="69" t="s">
         <v>92</v>
       </c>
@@ -10126,7 +10216,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="52" spans="1:30" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:30" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A52" s="69" t="s">
         <v>92</v>
       </c>
@@ -10170,12 +10260,12 @@
         <v>98</v>
       </c>
     </row>
-    <row r="54" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A54" s="70" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="55" spans="1:30" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:30" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A55" s="69" t="s">
         <v>676</v>
       </c>
@@ -10252,7 +10342,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="56" spans="1:30" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:30" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A56" s="69" t="s">
         <v>675</v>
       </c>
@@ -10329,7 +10419,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="57" spans="1:30" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:30" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A57" s="69" t="s">
         <v>675</v>
       </c>
@@ -10391,7 +10481,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="58" spans="1:30" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:30" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A58" s="69" t="s">
         <v>675</v>
       </c>
@@ -10453,12 +10543,12 @@
         <v>98</v>
       </c>
     </row>
-    <row r="61" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A61" s="6" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="62" spans="1:30" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:30" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A62" s="69" t="s">
         <v>115</v>
       </c>
@@ -10502,7 +10592,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="63" spans="1:30" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:30" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A63" s="69" t="s">
         <v>122</v>
       </c>
@@ -10551,12 +10641,12 @@
       <c r="AA63" s="74"/>
       <c r="AD63" s="74"/>
     </row>
-    <row r="66" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A66" s="6" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="67" spans="1:30" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:30" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A67" s="69" t="s">
         <v>115</v>
       </c>
@@ -10600,7 +10690,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="68" spans="1:30" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:30" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A68" s="69" t="s">
         <v>122</v>
       </c>
@@ -10649,7 +10739,7 @@
       <c r="AA68" s="74"/>
       <c r="AD68" s="74"/>
     </row>
-    <row r="71" spans="1:30" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:30" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A71" s="69" t="s">
         <v>72</v>
       </c>
@@ -10693,7 +10783,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="72" spans="1:30" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:30" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A72" s="69" t="s">
         <v>509</v>
       </c>
@@ -10737,13 +10827,13 @@
         <v>44</v>
       </c>
     </row>
-    <row r="74" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A74" s="49" t="s">
         <v>513</v>
       </c>
       <c r="M74" s="86"/>
     </row>
-    <row r="75" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A75" s="69" t="s">
         <v>49</v>
       </c>
@@ -10823,7 +10913,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="76" spans="1:30" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:30" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="75" t="s">
         <v>70</v>
       </c>
@@ -10903,13 +10993,13 @@
         <v>541</v>
       </c>
     </row>
-    <row r="78" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A78" s="49" t="s">
         <v>518</v>
       </c>
       <c r="M78" s="86"/>
     </row>
-    <row r="79" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A79" s="69" t="s">
         <v>49</v>
       </c>
@@ -10956,7 +11046,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="80" spans="1:30" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:30" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="75" t="s">
         <v>70</v>
       </c>
@@ -11003,13 +11093,13 @@
         <v>44</v>
       </c>
     </row>
-    <row r="82" spans="1:28" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:28" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A82" s="49" t="s">
         <v>543</v>
       </c>
       <c r="M82" s="86"/>
     </row>
-    <row r="83" spans="1:28" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:28" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="69" t="s">
         <v>49</v>
       </c>
@@ -11095,7 +11185,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="84" spans="1:28" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:28" ht="32.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" s="75" t="s">
         <v>70</v>
       </c>
@@ -11181,13 +11271,13 @@
         <v>544</v>
       </c>
     </row>
-    <row r="86" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A86" s="6" t="s">
         <v>549</v>
       </c>
       <c r="M86" s="92"/>
     </row>
-    <row r="87" spans="1:28" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:28" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A87" s="69" t="s">
         <v>643</v>
       </c>
@@ -11235,7 +11325,7 @@
       </c>
       <c r="Q87" s="33"/>
     </row>
-    <row r="88" spans="1:28" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:28" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A88" s="74" t="s">
         <v>652</v>
       </c>
@@ -11283,13 +11373,13 @@
       </c>
       <c r="Q88" s="33"/>
     </row>
-    <row r="91" spans="1:28" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:28" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A91" s="70" t="s">
         <v>581</v>
       </c>
       <c r="M91" s="86"/>
     </row>
-    <row r="92" spans="1:28" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:28" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A92" s="69" t="s">
         <v>642</v>
       </c>
@@ -11322,7 +11412,7 @@
       </c>
       <c r="N92" s="33"/>
     </row>
-    <row r="93" spans="1:28" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:28" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A93" s="74" t="s">
         <v>585</v>
       </c>
@@ -11355,13 +11445,13 @@
       </c>
       <c r="N93" s="33"/>
     </row>
-    <row r="96" spans="1:28" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:28" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A96" s="70" t="s">
         <v>594</v>
       </c>
       <c r="M96" s="86"/>
     </row>
-    <row r="97" spans="1:18" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:18" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A97" s="69" t="s">
         <v>657</v>
       </c>
@@ -11406,7 +11496,7 @@
       </c>
       <c r="R97" s="33"/>
     </row>
-    <row r="98" spans="1:18" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:18" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A98" s="74" t="s">
         <v>658</v>
       </c>
@@ -11451,13 +11541,13 @@
       </c>
       <c r="R98" s="33"/>
     </row>
-    <row r="101" spans="1:18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>665</v>
       </c>
       <c r="M101" s="17"/>
     </row>
-    <row r="102" spans="1:18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A102" s="49" t="s">
         <v>657</v>
       </c>
@@ -11466,7 +11556,7 @@
       </c>
       <c r="M102" s="17"/>
     </row>
-    <row r="103" spans="1:18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A103" s="72" t="s">
         <v>664</v>
       </c>
@@ -11493,37 +11583,37 @@
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" style="17" customWidth="1"/>
-    <col min="3" max="3" width="35.5703125" style="17" customWidth="1"/>
-    <col min="4" max="4" width="29.5703125" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.140625" style="17" customWidth="1"/>
-    <col min="6" max="6" width="28.42578125" style="17" customWidth="1"/>
-    <col min="7" max="7" width="30.42578125" style="17" customWidth="1"/>
-    <col min="8" max="8" width="43.140625" style="17" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.7109375" style="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.28515625" style="17" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="36.140625" style="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="40.7109375" style="17" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="30.5703125" style="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="39.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="40.85546875" style="17" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="39.140625" style="17" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="49.85546875" style="17" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="46.5703125" style="17" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="43.85546875" style="17" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.85546875" style="17" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="44.7109375" style="17" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="45.85546875" style="17" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="35.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.7109375" style="17"/>
-    <col min="25" max="26" width="41.5703125" style="17" bestFit="1" customWidth="1"/>
-    <col min="27" max="16384" width="8.7109375" style="17"/>
+    <col min="1" max="1" width="22.453125" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.81640625" style="17" customWidth="1"/>
+    <col min="3" max="3" width="35.54296875" style="17" customWidth="1"/>
+    <col min="4" max="4" width="29.54296875" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.1796875" style="17" customWidth="1"/>
+    <col min="6" max="6" width="28.453125" style="17" customWidth="1"/>
+    <col min="7" max="7" width="30.453125" style="17" customWidth="1"/>
+    <col min="8" max="8" width="43.1796875" style="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.7265625" style="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.26953125" style="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="36.1796875" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="40.7265625" style="17" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="30.54296875" style="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="39.453125" style="17" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="40.81640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="39.1796875" style="17" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="49.81640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="46.54296875" style="17" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="43.81640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.81640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="44.7265625" style="17" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="45.81640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="35.453125" style="17" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.7265625" style="17"/>
+    <col min="25" max="26" width="41.54296875" style="17" bestFit="1" customWidth="1"/>
+    <col min="27" max="16384" width="8.7265625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="40" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" s="40" customFormat="1" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="35" t="s">
         <v>391</v>
       </c>
@@ -11549,13 +11639,13 @@
         <v>393</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:23" s="42" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:23" s="42" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="41" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="4" spans="1:23" s="57" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" s="57" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="61" t="s">
         <v>174</v>
       </c>
@@ -11626,7 +11716,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="5" spans="1:23" s="44" customFormat="1" ht="26.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" s="44" customFormat="1" ht="26.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="43" t="s">
         <v>233</v>
       </c>
@@ -11697,13 +11787,13 @@
         <v>243</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:23" s="57" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" ht="32.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:23" s="57" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="56" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="8" spans="1:23" s="57" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" s="57" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="57" t="s">
         <v>142</v>
       </c>
@@ -11753,7 +11843,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="9" spans="1:23" s="59" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" s="59" customFormat="1" ht="96" x14ac:dyDescent="0.4">
       <c r="A9" s="59" t="s">
         <v>236</v>
       </c>
@@ -11809,12 +11899,12 @@
       <c r="U9" s="60"/>
       <c r="V9" s="60"/>
     </row>
-    <row r="12" spans="1:23" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="22" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="13" spans="1:23" s="21" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" s="21" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="21" t="s">
         <v>142</v>
       </c>
@@ -11885,7 +11975,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="14" spans="1:23" s="19" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" s="19" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A14" s="19" t="s">
         <v>236</v>
       </c>
@@ -11956,13 +12046,13 @@
         <v>249</v>
       </c>
     </row>
-    <row r="15" spans="1:23" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:23" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" ht="7.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:23" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="48" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:26" s="50" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" s="50" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" s="50" t="s">
         <v>72</v>
       </c>
@@ -12042,7 +12132,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="18" spans="1:26" s="52" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" s="52" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A18" s="52" t="s">
         <v>253</v>
       </c>
@@ -12129,29 +12219,30 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6D13D71-B365-458F-8758-84786862308D}">
-  <dimension ref="A1:G74"/>
+  <dimension ref="A1:G78"/>
   <sheetViews>
-    <sheetView topLeftCell="B72" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F72" sqref="F72"/>
+    <sheetView topLeftCell="A75" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="35.5" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" style="17" customWidth="1"/>
-    <col min="2" max="2" width="27.140625" style="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.5703125" style="101" customWidth="1"/>
-    <col min="4" max="4" width="69.85546875" style="17" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" style="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="47.5703125" style="101" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.7109375" style="17"/>
+    <col min="1" max="1" width="10.54296875" style="17" customWidth="1"/>
+    <col min="2" max="2" width="27.1796875" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.54296875" style="101" customWidth="1"/>
+    <col min="4" max="4" width="69.81640625" style="17" customWidth="1"/>
+    <col min="5" max="5" width="21.7265625" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="87.453125" style="101" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.7265625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D1" s="114" t="s">
         <v>600</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="87" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="87" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="87" t="s">
         <v>419</v>
       </c>
@@ -12171,7 +12262,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="32" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="32" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="32" t="s">
         <v>420</v>
       </c>
@@ -12189,7 +12280,7 @@
       </c>
       <c r="F3" s="103"/>
     </row>
-    <row r="4" spans="1:6" s="32" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" s="32" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="32" t="s">
         <v>421</v>
       </c>
@@ -12207,7 +12298,7 @@
       </c>
       <c r="F4" s="103"/>
     </row>
-    <row r="5" spans="1:6" s="32" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" s="32" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="32" t="s">
         <v>422</v>
       </c>
@@ -12225,7 +12316,7 @@
       </c>
       <c r="F5" s="103"/>
     </row>
-    <row r="6" spans="1:6" s="32" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" s="32" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="32" t="s">
         <v>423</v>
       </c>
@@ -12243,7 +12334,7 @@
       </c>
       <c r="F6" s="103"/>
     </row>
-    <row r="7" spans="1:6" s="32" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" s="32" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="32" t="s">
         <v>424</v>
       </c>
@@ -12261,7 +12352,7 @@
       </c>
       <c r="F7" s="103"/>
     </row>
-    <row r="8" spans="1:6" s="32" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" s="32" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="32" t="s">
         <v>425</v>
       </c>
@@ -12279,12 +12370,12 @@
       </c>
       <c r="F8" s="103"/>
     </row>
-    <row r="10" spans="1:6" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D10" s="114" t="s">
         <v>599</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="87" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" s="87" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="87" t="s">
         <v>419</v>
       </c>
@@ -12304,7 +12395,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="32" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" s="32" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="32" t="s">
         <v>426</v>
       </c>
@@ -12322,7 +12413,7 @@
       </c>
       <c r="F12" s="103"/>
     </row>
-    <row r="13" spans="1:6" s="32" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" s="32" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="32" t="s">
         <v>427</v>
       </c>
@@ -12340,7 +12431,7 @@
       </c>
       <c r="F13" s="103"/>
     </row>
-    <row r="14" spans="1:6" s="32" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" s="32" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="32" t="s">
         <v>428</v>
       </c>
@@ -12358,7 +12449,7 @@
       </c>
       <c r="F14" s="103"/>
     </row>
-    <row r="15" spans="1:6" s="32" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" s="32" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="32" t="s">
         <v>429</v>
       </c>
@@ -12376,7 +12467,7 @@
       </c>
       <c r="F15" s="103"/>
     </row>
-    <row r="16" spans="1:6" s="32" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" s="32" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="32" t="s">
         <v>430</v>
       </c>
@@ -12394,7 +12485,7 @@
       </c>
       <c r="F16" s="103"/>
     </row>
-    <row r="17" spans="1:6" s="32" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" s="32" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="32" t="s">
         <v>431</v>
       </c>
@@ -12412,7 +12503,7 @@
       </c>
       <c r="F17" s="103"/>
     </row>
-    <row r="18" spans="1:6" s="32" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" s="32" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="32" t="s">
         <v>432</v>
       </c>
@@ -12430,7 +12521,7 @@
       </c>
       <c r="F18" s="103"/>
     </row>
-    <row r="19" spans="1:6" s="32" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" s="32" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="32" t="s">
         <v>433</v>
       </c>
@@ -12448,7 +12539,7 @@
       </c>
       <c r="F19" s="103"/>
     </row>
-    <row r="20" spans="1:6" s="32" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" s="32" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="32" t="s">
         <v>434</v>
       </c>
@@ -12466,7 +12557,7 @@
       </c>
       <c r="F20" s="103"/>
     </row>
-    <row r="21" spans="1:6" s="32" customFormat="1" ht="39" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" s="32" customFormat="1" ht="39.5" x14ac:dyDescent="0.35">
       <c r="A21" s="32" t="s">
         <v>435</v>
       </c>
@@ -12481,15 +12572,15 @@
       </c>
       <c r="F21" s="103"/>
     </row>
-    <row r="22" spans="1:6" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="32"/>
     </row>
-    <row r="24" spans="1:6" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D24" s="114" t="s">
         <v>598</v>
       </c>
     </row>
-    <row r="25" spans="1:6" s="87" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" s="87" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="87" t="s">
         <v>419</v>
       </c>
@@ -12509,7 +12600,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="32" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" s="32" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="32" t="s">
         <v>436</v>
       </c>
@@ -12529,7 +12620,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="32" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" s="32" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="32" t="s">
         <v>437</v>
       </c>
@@ -12547,7 +12638,7 @@
       </c>
       <c r="F27" s="103"/>
     </row>
-    <row r="28" spans="1:6" s="32" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" s="32" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="32" t="s">
         <v>438</v>
       </c>
@@ -12565,7 +12656,7 @@
       </c>
       <c r="F28" s="103"/>
     </row>
-    <row r="29" spans="1:6" s="32" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" s="32" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="32" t="s">
         <v>439</v>
       </c>
@@ -12583,7 +12674,7 @@
       </c>
       <c r="F29" s="103"/>
     </row>
-    <row r="30" spans="1:6" s="32" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" s="32" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="32" t="s">
         <v>440</v>
       </c>
@@ -12601,7 +12692,7 @@
       </c>
       <c r="F30" s="103"/>
     </row>
-    <row r="31" spans="1:6" s="32" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" s="32" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="32" t="s">
         <v>441</v>
       </c>
@@ -12619,7 +12710,7 @@
       </c>
       <c r="F31" s="103"/>
     </row>
-    <row r="32" spans="1:6" s="32" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" s="32" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="32" t="s">
         <v>442</v>
       </c>
@@ -12637,7 +12728,7 @@
       </c>
       <c r="F32" s="103"/>
     </row>
-    <row r="33" spans="1:6" s="32" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" s="32" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="32" t="s">
         <v>443</v>
       </c>
@@ -12655,7 +12746,7 @@
       </c>
       <c r="F33" s="103"/>
     </row>
-    <row r="34" spans="1:6" s="32" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" s="32" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="32" t="s">
         <v>444</v>
       </c>
@@ -12673,7 +12764,7 @@
       </c>
       <c r="F34" s="103"/>
     </row>
-    <row r="35" spans="1:6" s="32" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" s="32" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="32" t="s">
         <v>445</v>
       </c>
@@ -12691,7 +12782,7 @@
       </c>
       <c r="F35" s="103"/>
     </row>
-    <row r="36" spans="1:6" s="32" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" s="32" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="32" t="s">
         <v>446</v>
       </c>
@@ -12709,7 +12800,7 @@
       </c>
       <c r="F36" s="103"/>
     </row>
-    <row r="37" spans="1:6" s="32" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" s="32" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="32" t="s">
         <v>447</v>
       </c>
@@ -12727,7 +12818,7 @@
       </c>
       <c r="F37" s="103"/>
     </row>
-    <row r="38" spans="1:6" s="32" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" s="32" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="32" t="s">
         <v>448</v>
       </c>
@@ -12745,7 +12836,7 @@
       </c>
       <c r="F38" s="103"/>
     </row>
-    <row r="39" spans="1:6" s="32" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" s="32" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="32" t="s">
         <v>449</v>
       </c>
@@ -12763,12 +12854,12 @@
       </c>
       <c r="F39" s="103"/>
     </row>
-    <row r="40" spans="1:6" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D40" s="114" t="s">
         <v>597</v>
       </c>
     </row>
-    <row r="41" spans="1:6" s="87" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" s="87" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="87" t="s">
         <v>419</v>
       </c>
@@ -12786,7 +12877,7 @@
       </c>
       <c r="F41" s="99"/>
     </row>
-    <row r="42" spans="1:6" s="32" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" s="32" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A42" s="32" t="s">
         <v>450</v>
       </c>
@@ -12804,7 +12895,7 @@
       </c>
       <c r="F42" s="103"/>
     </row>
-    <row r="43" spans="1:6" s="32" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" s="32" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="32" t="s">
         <v>451</v>
       </c>
@@ -12822,7 +12913,7 @@
       </c>
       <c r="F43" s="103"/>
     </row>
-    <row r="44" spans="1:6" s="32" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" s="32" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="32" t="s">
         <v>452</v>
       </c>
@@ -12840,7 +12931,7 @@
       </c>
       <c r="F44" s="103"/>
     </row>
-    <row r="45" spans="1:6" s="32" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" s="32" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="32" t="s">
         <v>453</v>
       </c>
@@ -12858,7 +12949,7 @@
       </c>
       <c r="F45" s="103"/>
     </row>
-    <row r="46" spans="1:6" s="32" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" s="32" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="32" t="s">
         <v>454</v>
       </c>
@@ -12876,7 +12967,7 @@
       </c>
       <c r="F46" s="103"/>
     </row>
-    <row r="47" spans="1:6" s="32" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" s="32" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="32" t="s">
         <v>455</v>
       </c>
@@ -12894,12 +12985,12 @@
       </c>
       <c r="F47" s="103"/>
     </row>
-    <row r="48" spans="1:6" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D48" s="114" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="49" spans="1:7" s="24" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" s="24" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="24" t="s">
         <v>419</v>
       </c>
@@ -12917,7 +13008,7 @@
       </c>
       <c r="F49" s="102"/>
     </row>
-    <row r="50" spans="1:7" s="18" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" s="18" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="32" t="s">
         <v>468</v>
       </c>
@@ -12935,7 +13026,7 @@
       </c>
       <c r="F50" s="107"/>
     </row>
-    <row r="51" spans="1:7" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" s="18" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A51" s="32" t="s">
         <v>469</v>
       </c>
@@ -12953,7 +13044,7 @@
       </c>
       <c r="F51" s="107"/>
     </row>
-    <row r="52" spans="1:7" s="18" customFormat="1" ht="46.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" s="18" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A52" s="32" t="s">
         <v>470</v>
       </c>
@@ -12971,7 +13062,7 @@
       </c>
       <c r="F52" s="107"/>
     </row>
-    <row r="53" spans="1:7" s="18" customFormat="1" ht="61.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" s="18" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A53" s="32" t="s">
         <v>471</v>
       </c>
@@ -12989,7 +13080,7 @@
       </c>
       <c r="F53" s="107"/>
     </row>
-    <row r="54" spans="1:7" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" s="18" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A54" s="32" t="s">
         <v>482</v>
       </c>
@@ -13007,7 +13098,7 @@
       </c>
       <c r="F54" s="107"/>
     </row>
-    <row r="55" spans="1:7" s="91" customFormat="1" ht="46.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" s="91" customFormat="1" ht="45" x14ac:dyDescent="0.35">
       <c r="A55" s="88" t="s">
         <v>483</v>
       </c>
@@ -13025,7 +13116,7 @@
       </c>
       <c r="F55" s="108"/>
     </row>
-    <row r="56" spans="1:7" s="18" customFormat="1" ht="46.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" s="18" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A56" s="32" t="s">
         <v>484</v>
       </c>
@@ -13043,7 +13134,7 @@
       </c>
       <c r="F56" s="107"/>
     </row>
-    <row r="57" spans="1:7" s="18" customFormat="1" ht="46.5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" s="18" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A57" s="32" t="s">
         <v>494</v>
       </c>
@@ -13061,19 +13152,19 @@
       </c>
       <c r="F57" s="107"/>
     </row>
-    <row r="58" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A58" s="112"/>
       <c r="B58" s="113"/>
       <c r="C58" s="104"/>
       <c r="D58" s="92"/>
       <c r="E58" s="113"/>
     </row>
-    <row r="59" spans="1:7" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D59" s="114" t="s">
         <v>595</v>
       </c>
     </row>
-    <row r="60" spans="1:7" s="24" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" s="24" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="24" t="s">
         <v>419</v>
       </c>
@@ -13096,7 +13187,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="61" spans="1:7" s="18" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" s="18" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="32" t="s">
         <v>566</v>
       </c>
@@ -13116,7 +13207,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="62" spans="1:7" s="18" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" s="18" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="18" t="s">
         <v>572</v>
       </c>
@@ -13136,7 +13227,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="63" spans="1:7" s="18" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" s="18" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="18" t="s">
         <v>578</v>
       </c>
@@ -13156,7 +13247,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="64" spans="1:7" s="18" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" s="18" customFormat="1" ht="116" x14ac:dyDescent="0.35">
       <c r="A64" s="18" t="s">
         <v>591</v>
       </c>
@@ -13176,7 +13267,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="65" spans="1:7" s="18" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" s="18" customFormat="1" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A65" s="18" t="s">
         <v>592</v>
       </c>
@@ -13196,7 +13287,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="17" t="s">
         <v>616</v>
       </c>
@@ -13213,12 +13304,12 @@
         <v>567</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D67" s="114" t="s">
         <v>612</v>
       </c>
     </row>
-    <row r="68" spans="1:7" s="24" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" s="24" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="24" t="s">
         <v>419</v>
       </c>
@@ -13241,7 +13332,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A69" s="18" t="s">
         <v>592</v>
       </c>
@@ -13261,7 +13352,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="18" t="s">
         <v>603</v>
       </c>
@@ -13281,7 +13372,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="18" t="s">
         <v>610</v>
       </c>
@@ -13301,7 +13392,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="18" t="s">
         <v>611</v>
       </c>
@@ -13318,7 +13409,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A73" s="18" t="s">
         <v>624</v>
       </c>
@@ -13338,7 +13429,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" ht="116" x14ac:dyDescent="0.35">
       <c r="A74" s="18" t="s">
         <v>624</v>
       </c>
@@ -13356,6 +13447,57 @@
       </c>
       <c r="F74" s="101" t="s">
         <v>628</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D76" s="114" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" s="24" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="24" t="s">
+        <v>419</v>
+      </c>
+      <c r="B77" s="24" t="s">
+        <v>286</v>
+      </c>
+      <c r="C77" s="102" t="s">
+        <v>275</v>
+      </c>
+      <c r="D77" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="E77" s="24" t="s">
+        <v>357</v>
+      </c>
+      <c r="F77" s="102" t="s">
+        <v>575</v>
+      </c>
+      <c r="G77" s="24" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="17" t="s">
+        <v>686</v>
+      </c>
+      <c r="B78" s="117" t="s">
+        <v>288</v>
+      </c>
+      <c r="C78" s="118" t="s">
+        <v>685</v>
+      </c>
+      <c r="D78" s="17" t="s">
+        <v>687</v>
+      </c>
+      <c r="E78" s="117" t="s">
+        <v>288</v>
+      </c>
+      <c r="F78" s="69" t="s">
+        <v>688</v>
+      </c>
+      <c r="G78" s="17" t="s">
+        <v>690</v>
       </c>
     </row>
   </sheetData>
@@ -13372,15 +13514,15 @@
       <selection activeCell="AG65" sqref="AG65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>56</v>
       </c>
       <c r="M2" s="92"/>
     </row>
-    <row r="3" spans="1:35" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>72</v>
       </c>
@@ -13460,7 +13602,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="4" spans="1:35" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>73</v>
       </c>
@@ -13540,21 +13682,21 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
       <c r="M5" s="17"/>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
       <c r="M6" s="17"/>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
       <c r="M7" s="17"/>
     </row>
-    <row r="8" spans="1:35" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="63" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="9" spans="1:35" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" s="7" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>142</v>
       </c>
@@ -13637,7 +13779,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="10" spans="1:35" s="7" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" s="7" customFormat="1" ht="116" x14ac:dyDescent="0.35">
       <c r="A10" s="49" t="s">
         <v>551</v>
       </c>
@@ -13720,22 +13862,22 @@
         <v>662</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.35">
       <c r="M11" s="17"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
       <c r="M12" s="17"/>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
       <c r="M13" s="17"/>
     </row>
-    <row r="14" spans="1:35" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" s="30" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="30" t="s">
         <v>316</v>
       </c>
       <c r="M14" s="93"/>
     </row>
-    <row r="15" spans="1:35" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" s="2" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>174</v>
       </c>
@@ -13842,7 +13984,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="16" spans="1:35" s="2" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" s="2" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>387</v>
       </c>
@@ -13949,16 +14091,16 @@
         <v>383</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.35">
       <c r="M17" s="17"/>
     </row>
-    <row r="18" spans="1:35" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" s="30" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="30" t="s">
         <v>385</v>
       </c>
       <c r="M18" s="93"/>
     </row>
-    <row r="19" spans="1:35" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:35" s="2" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>174</v>
       </c>
@@ -14065,7 +14207,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="20" spans="1:35" s="2" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35" s="2" customFormat="1" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>386</v>
       </c>
@@ -14172,16 +14314,16 @@
         <v>383</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.35">
       <c r="M21" s="17"/>
     </row>
-    <row r="22" spans="1:35" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:35" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="70" t="s">
         <v>69</v>
       </c>
       <c r="M22" s="86"/>
     </row>
-    <row r="23" spans="1:35" s="69" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:35" s="69" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="69" t="s">
         <v>72</v>
       </c>
@@ -14225,7 +14367,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:35" s="69" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:35" s="69" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A24" s="69" t="s">
         <v>73</v>
       </c>
@@ -14269,7 +14411,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:35" s="69" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:35" s="69" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A25" s="69" t="s">
         <v>73</v>
       </c>
@@ -14313,7 +14455,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:35" s="69" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:35" s="69" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A26" s="69" t="s">
         <v>73</v>
       </c>
@@ -14357,16 +14499,16 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.35">
       <c r="M27" s="17"/>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A28" s="81" t="s">
         <v>406</v>
       </c>
       <c r="M28" s="17"/>
     </row>
-    <row r="29" spans="1:35" s="69" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:35" s="69" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="69" t="s">
         <v>72</v>
       </c>
@@ -14410,7 +14552,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:35" s="69" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:35" s="69" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A30" s="69" t="s">
         <v>73</v>
       </c>
@@ -14454,23 +14596,23 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.35">
       <c r="M31" s="17"/>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A32" s="5"/>
       <c r="M32" s="17"/>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.35">
       <c r="M33" s="17"/>
     </row>
-    <row r="34" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="70" t="s">
         <v>407</v>
       </c>
       <c r="M34" s="86"/>
     </row>
-    <row r="35" spans="1:30" s="69" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:30" s="69" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A35" s="69" t="s">
         <v>99</v>
       </c>
@@ -14523,7 +14665,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:30" s="69" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:30" s="69" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="69" t="s">
         <v>92</v>
       </c>
@@ -14576,19 +14718,19 @@
         <v>78</v>
       </c>
     </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:30" x14ac:dyDescent="0.35">
       <c r="M37" s="17"/>
     </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:30" x14ac:dyDescent="0.35">
       <c r="M38" s="17"/>
     </row>
-    <row r="39" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="70" t="s">
         <v>458</v>
       </c>
       <c r="M39" s="86"/>
     </row>
-    <row r="40" spans="1:30" s="69" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:30" s="69" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A40" s="69" t="s">
         <v>99</v>
       </c>
@@ -14644,7 +14786,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="41" spans="1:30" s="69" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:30" s="69" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A41" s="69" t="s">
         <v>92</v>
       </c>
@@ -14700,16 +14842,16 @@
         <v>87</v>
       </c>
     </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:30" x14ac:dyDescent="0.35">
       <c r="M42" s="17"/>
     </row>
-    <row r="43" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A43" s="6" t="s">
         <v>462</v>
       </c>
       <c r="M43" s="86"/>
     </row>
-    <row r="44" spans="1:30" s="69" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:30" s="69" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A44" s="69" t="s">
         <v>115</v>
       </c>
@@ -14753,7 +14895,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="45" spans="1:30" s="69" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:30" s="69" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A45" s="69" t="s">
         <v>122</v>
       </c>
@@ -14802,19 +14944,19 @@
       <c r="AA45" s="74"/>
       <c r="AD45" s="74"/>
     </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:30" x14ac:dyDescent="0.35">
       <c r="M46" s="17"/>
     </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:30" x14ac:dyDescent="0.35">
       <c r="M47" s="17"/>
     </row>
-    <row r="48" spans="1:30" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:30" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A48" s="6" t="s">
         <v>488</v>
       </c>
       <c r="M48" s="18"/>
     </row>
-    <row r="49" spans="1:30" s="69" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:30" s="69" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A49" s="69" t="s">
         <v>115</v>
       </c>
@@ -14858,7 +15000,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="50" spans="1:30" s="69" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:30" s="69" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A50" s="69" t="s">
         <v>122</v>
       </c>
@@ -14907,16 +15049,16 @@
       <c r="AA50" s="74"/>
       <c r="AD50" s="74"/>
     </row>
-    <row r="51" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:30" x14ac:dyDescent="0.35">
       <c r="M51" s="17"/>
     </row>
-    <row r="52" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A52" s="49" t="s">
         <v>178</v>
       </c>
       <c r="M52" s="86"/>
     </row>
-    <row r="53" spans="1:30" s="69" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:30" s="69" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A53" s="69" t="s">
         <v>174</v>
       </c>
@@ -14999,7 +15141,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="54" spans="1:30" s="69" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:30" s="69" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A54" s="74" t="s">
         <v>507</v>
       </c>
@@ -15082,16 +15224,16 @@
         <v>332</v>
       </c>
     </row>
-    <row r="55" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:30" x14ac:dyDescent="0.35">
       <c r="M55" s="17"/>
     </row>
-    <row r="56" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A56" s="49" t="s">
         <v>513</v>
       </c>
       <c r="M56" s="86"/>
     </row>
-    <row r="57" spans="1:30" s="29" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:30" s="29" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A57" s="69" t="s">
         <v>49</v>
       </c>
@@ -15173,7 +15315,7 @@
       <c r="AA57" s="69"/>
       <c r="AB57" s="69"/>
     </row>
-    <row r="58" spans="1:30" s="29" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:30" s="29" customFormat="1" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="75" t="s">
         <v>70</v>
       </c>
@@ -15255,16 +15397,16 @@
       <c r="AA58" s="69"/>
       <c r="AB58" s="69"/>
     </row>
-    <row r="59" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:30" x14ac:dyDescent="0.35">
       <c r="M59" s="17"/>
     </row>
-    <row r="60" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A60" s="49" t="s">
         <v>518</v>
       </c>
       <c r="M60" s="86"/>
     </row>
-    <row r="61" spans="1:30" s="29" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:30" s="29" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A61" s="69" t="s">
         <v>49</v>
       </c>
@@ -15311,7 +15453,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="62" spans="1:30" s="29" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:30" s="29" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="75" t="s">
         <v>70</v>
       </c>
@@ -15358,16 +15500,16 @@
         <v>44</v>
       </c>
     </row>
-    <row r="63" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:30" x14ac:dyDescent="0.35">
       <c r="M63" s="17"/>
     </row>
-    <row r="64" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A64" s="49" t="s">
         <v>543</v>
       </c>
       <c r="M64" s="86"/>
     </row>
-    <row r="65" spans="1:28" s="29" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:28" s="29" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="69" t="s">
         <v>49</v>
       </c>
@@ -15453,7 +15595,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="66" spans="1:28" s="29" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:28" s="29" customFormat="1" ht="32.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="75" t="s">
         <v>70</v>
       </c>
@@ -15539,16 +15681,16 @@
         <v>544</v>
       </c>
     </row>
-    <row r="67" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:28" x14ac:dyDescent="0.35">
       <c r="M67" s="17"/>
     </row>
-    <row r="68" spans="1:28" s="73" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:28" s="73" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A68" s="82" t="s">
         <v>549</v>
       </c>
       <c r="M68" s="94"/>
     </row>
-    <row r="69" spans="1:28" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:28" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A69" s="49" t="s">
         <v>643</v>
       </c>
@@ -15596,7 +15738,7 @@
       </c>
       <c r="Q69" s="86"/>
     </row>
-    <row r="70" spans="1:28" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:28" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A70" s="72" t="s">
         <v>644</v>
       </c>
@@ -15644,19 +15786,19 @@
       </c>
       <c r="Q70" s="86"/>
     </row>
-    <row r="71" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:28" x14ac:dyDescent="0.35">
       <c r="M71" s="17"/>
     </row>
-    <row r="72" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:28" x14ac:dyDescent="0.35">
       <c r="L72" s="17"/>
     </row>
-    <row r="73" spans="1:28" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:28" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A73" s="70" t="s">
         <v>594</v>
       </c>
       <c r="M73" s="86"/>
     </row>
-    <row r="74" spans="1:28" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:28" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A74" s="69" t="s">
         <v>657</v>
       </c>
@@ -15701,7 +15843,7 @@
       </c>
       <c r="R74" s="33"/>
     </row>
-    <row r="75" spans="1:28" s="69" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:28" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A75" s="74" t="s">
         <v>658</v>
       </c>
@@ -15746,16 +15888,16 @@
       </c>
       <c r="R75" s="33"/>
     </row>
-    <row r="76" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:28" x14ac:dyDescent="0.35">
       <c r="M76" s="17"/>
     </row>
-    <row r="77" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>665</v>
       </c>
       <c r="M77" s="17"/>
     </row>
-    <row r="78" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A78" s="49" t="s">
         <v>657</v>
       </c>
@@ -15764,7 +15906,7 @@
       </c>
       <c r="M78" s="17"/>
     </row>
-    <row r="79" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A79" s="72" t="s">
         <v>667</v>
       </c>
@@ -15773,7 +15915,7 @@
       </c>
       <c r="M79" s="17"/>
     </row>
-    <row r="80" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:28" x14ac:dyDescent="0.35">
       <c r="M80" s="17"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data base testing code updated
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/Test_Data_Sheet.xlsx
+++ b/src/test/resources/testdata/Test_Data_Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sunil\eclipse-workspace\Regression_Pos_project\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C054429F-A688-4FD5-B9AA-C6DA775CF095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCD045B6-8817-45F9-B28F-645923CD01B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="751" xr2:uid="{52826312-55BE-45F7-9B29-2F6A9A52A5DF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="751" activeTab="2" xr2:uid="{52826312-55BE-45F7-9B29-2F6A9A52A5DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="2" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4729" uniqueCount="751">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4703" uniqueCount="748">
   <si>
     <t>admin</t>
   </si>
@@ -2607,15 +2607,6 @@
   </si>
   <si>
     <t>Lekha</t>
-  </si>
-  <si>
-    <t>Inventory List Search Data for Adjustment</t>
-  </si>
-  <si>
-    <t>25001200</t>
-  </si>
-  <si>
-    <t>8904389900611</t>
   </si>
   <si>
     <t>2025-01-15 04:51 pm</t>
@@ -3725,10 +3716,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3759,122 +3750,39 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B2" s="119" t="s">
-        <v>678</v>
+      <c r="B2" s="126" t="s">
+        <v>545</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>61</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B3" s="9" t="s">
-        <v>511</v>
+      <c r="B3" s="126" t="s">
+        <v>144</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="11" t="s">
-        <v>61</v>
-      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B4" s="9" t="s">
-        <v>539</v>
+      <c r="B4" s="117" t="s">
+        <v>590</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B5" s="9" t="s">
-        <v>487</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>675</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B6" s="9" t="s">
-        <v>461</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>61</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B7" s="117" t="s">
-        <v>457</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>675</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B8" s="9" t="s">
-        <v>406</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B9" s="9" t="s">
-        <v>405</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B10" s="9" t="s">
-        <v>699</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B11" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>61</v>
-      </c>
+      <c r="B7" s="117"/>
     </row>
   </sheetData>
   <autoFilter ref="C1" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1 E2:E1048576" xr:uid="{AEBF9179-D691-4AFE-9C0F-7B9ECE5923E0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576" xr:uid="{AEBF9179-D691-4AFE-9C0F-7B9ECE5923E0}">
       <formula1>"Complete,Inprogress,Non-Started"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1 C2:C1048576" xr:uid="{0B33546C-2E36-4AF5-B702-4D0334972A35}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{0B33546C-2E36-4AF5-B702-4D0334972A35}">
       <formula1>"Y,N"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5875,7 +5783,7 @@
   <dimension ref="A1:U35"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:M11"/>
+      <selection activeCell="I14" sqref="I14:M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6591,8 +6499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AD52"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="W11" sqref="W11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6622,13 +6530,13 @@
     <col min="25" max="27" width="42.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="49" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:27" s="49" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="70" t="s">
         <v>590</v>
       </c>
       <c r="M1" s="86"/>
     </row>
-    <row r="2" spans="1:28" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:27" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="69" t="s">
         <v>653</v>
       </c>
@@ -6673,7 +6581,7 @@
       </c>
       <c r="R2" s="33"/>
     </row>
-    <row r="3" spans="1:28" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:27" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="74" t="s">
         <v>654</v>
       </c>
@@ -6718,13 +6626,13 @@
       </c>
       <c r="R3" s="33"/>
     </row>
-    <row r="5" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:27" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>545</v>
       </c>
       <c r="M5" s="92"/>
     </row>
-    <row r="6" spans="1:28" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:27" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="69" t="s">
         <v>639</v>
       </c>
@@ -6772,7 +6680,7 @@
       </c>
       <c r="Q6" s="33"/>
     </row>
-    <row r="7" spans="1:28" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:27" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="74" t="s">
         <v>657</v>
       </c>
@@ -6820,191 +6728,184 @@
       </c>
       <c r="Q7" s="33"/>
     </row>
-    <row r="9" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:27" s="25" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="63" t="s">
         <v>144</v>
       </c>
-      <c r="M9" s="92"/>
-    </row>
-    <row r="10" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
+    </row>
+    <row r="10" spans="1:27" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="I10" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="J10" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="K10" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="L10" s="2" t="s">
+      <c r="L10" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="M10" s="23" t="s">
+      <c r="M10" s="92" t="s">
         <v>156</v>
       </c>
-      <c r="N10" s="2" t="s">
+      <c r="N10" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="O10" s="2" t="s">
+      <c r="O10" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="P10" s="2" t="s">
+      <c r="P10" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="Q10" s="2" t="s">
+      <c r="Q10" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="R10" s="2" t="s">
+      <c r="R10" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="S10" s="2" t="s">
+      <c r="S10" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="T10" s="2" t="s">
+      <c r="T10" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="U10" s="2" t="s">
+      <c r="U10" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="V10" s="2" t="s">
+      <c r="V10" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="W10" s="2" t="s">
+      <c r="W10" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="X10" s="2" t="s">
+      <c r="X10" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="Y10" s="2" t="s">
+      <c r="Y10" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="Z10" s="2" t="s">
+      <c r="Z10" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="AA10" s="2" t="s">
+      <c r="AA10" s="7" t="s">
         <v>211</v>
       </c>
-      <c r="AB10" s="2" t="s">
-        <v>746</v>
-      </c>
-    </row>
-    <row r="11" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11" s="2" t="s">
+    </row>
+    <row r="11" spans="1:27" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="49" t="s">
+        <v>547</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>525</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="7" t="s">
         <v>525</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="H11" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I11" s="2" t="s">
+      <c r="H11" s="49" t="s">
+        <v>547</v>
+      </c>
+      <c r="I11" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="J11" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="K11" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="L11" s="2" t="s">
+      <c r="L11" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="M11" s="23" t="s">
+      <c r="M11" s="92" t="s">
         <v>160</v>
       </c>
-      <c r="N11" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="O11" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="P11" s="4" t="s">
+      <c r="N11" s="72" t="s">
+        <v>208</v>
+      </c>
+      <c r="O11" s="49" t="s">
+        <v>547</v>
+      </c>
+      <c r="P11" s="98" t="s">
         <v>188</v>
       </c>
-      <c r="Q11" s="2" t="s">
+      <c r="Q11" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="R11" s="2" t="s">
+      <c r="R11" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="S11" s="4" t="s">
-        <v>544</v>
-      </c>
-      <c r="T11" s="4" t="s">
-        <v>747</v>
-      </c>
-      <c r="U11" s="4" t="s">
-        <v>748</v>
-      </c>
-      <c r="V11" s="4" t="s">
-        <v>738</v>
-      </c>
-      <c r="W11" s="4" t="s">
-        <v>737</v>
-      </c>
-      <c r="X11" s="4" t="s">
+      <c r="S11" s="72" t="s">
+        <v>163</v>
+      </c>
+      <c r="T11" s="72" t="s">
+        <v>164</v>
+      </c>
+      <c r="U11" s="72" t="s">
+        <v>164</v>
+      </c>
+      <c r="V11" s="72" t="s">
+        <v>164</v>
+      </c>
+      <c r="W11" s="72" t="s">
+        <v>164</v>
+      </c>
+      <c r="X11" s="72" t="s">
         <v>654</v>
       </c>
-      <c r="Y11" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="Z11" s="4" t="s">
-        <v>648</v>
-      </c>
-      <c r="AA11" s="4" t="s">
-        <v>658</v>
-      </c>
-      <c r="AB11" s="4" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="13" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="Y11" s="72" t="s">
+        <v>164</v>
+      </c>
+      <c r="Z11" s="72" t="s">
+        <v>208</v>
+      </c>
+      <c r="AA11" s="72" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>678</v>
       </c>
       <c r="M13" s="92"/>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>698</v>
       </c>
@@ -7034,7 +6935,7 @@
       </c>
       <c r="O14" s="17"/>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>697</v>
       </c>
@@ -7946,7 +7847,7 @@
         <v>72</v>
       </c>
       <c r="D43" s="69" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
       <c r="E43" s="80" t="s">
         <v>404</v>
@@ -7955,13 +7856,13 @@
         <v>700</v>
       </c>
       <c r="G43" s="75" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="H43" s="74" t="s">
         <v>77</v>
       </c>
       <c r="I43" s="69" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
       <c r="J43" s="69" t="s">
         <v>82</v>
@@ -9002,8 +8903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF6A61A0-E1EB-4236-B550-B929F046F19F}">
   <dimension ref="A1:AL92"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11915,8 +11816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{579C09BE-0AA8-4E72-B77C-C9E1EC3B70FC}">
   <dimension ref="A1:AL108"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="A98" sqref="A98:XFD99"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Mobile automation coe changes
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/Test_Data_Sheet.xlsx
+++ b/src/test/resources/testdata/Test_Data_Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sunil\eclipse-workspace\Regression_Pos_project\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A83413E-D2C6-4C3B-A362-CBCA128932F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23029C7E-50F3-4040-B027-09223CBDC36B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="751" xr2:uid="{52826312-55BE-45F7-9B29-2F6A9A52A5DF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="751" firstSheet="1" activeTab="2" xr2:uid="{52826312-55BE-45F7-9B29-2F6A9A52A5DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Test Cases'!$C$1:$C$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -50,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4829" uniqueCount="783">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4844" uniqueCount="794">
   <si>
     <t>admin</t>
   </si>
@@ -2718,7 +2717,40 @@
     <t>Void_Transaction_Report_TestCases</t>
   </si>
   <si>
-    <t>10011060110</t>
+    <t>10011050133</t>
+  </si>
+  <si>
+    <t>MposLoginTest</t>
+  </si>
+  <si>
+    <t>Mobile_Number_For_Login</t>
+  </si>
+  <si>
+    <t>7975331947</t>
+  </si>
+  <si>
+    <t>Select Store Name to Login</t>
+  </si>
+  <si>
+    <t>RDEP HSR</t>
+  </si>
+  <si>
+    <t>StoreCode_DB_Validation</t>
+  </si>
+  <si>
+    <t>SKU_DB_Validation</t>
+  </si>
+  <si>
+    <t>1555678</t>
+  </si>
+  <si>
+    <t>Test Case1</t>
+  </si>
+  <si>
+    <t>Transaction Flow Check</t>
+  </si>
+  <si>
+    <t>Mobile Number for Customer Details</t>
   </si>
 </sst>
 </file>
@@ -3191,7 +3223,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -3469,6 +3501,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3487,12 +3525,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3828,10 +3861,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3865,7 +3898,7 @@
       <c r="A2" s="8">
         <v>2</v>
       </c>
-      <c r="B2" s="133" t="s">
+      <c r="B2" s="127" t="s">
         <v>766</v>
       </c>
       <c r="C2" s="10" t="s">
@@ -3893,11 +3926,11 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B4" s="133" t="s">
+      <c r="B4" s="127" t="s">
         <v>770</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>172</v>
+        <v>66</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>61</v>
@@ -3911,7 +3944,7 @@
         <v>777</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>172</v>
+        <v>66</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>61</v>
@@ -3925,7 +3958,7 @@
         <v>778</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>172</v>
+        <v>66</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>61</v>
@@ -3935,11 +3968,11 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B7" s="134" t="s">
+      <c r="B7" s="128" t="s">
         <v>779</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>172</v>
+        <v>66</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>61</v>
@@ -3953,7 +3986,7 @@
         <v>780</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>172</v>
+        <v>66</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>61</v>
@@ -3967,13 +4000,21 @@
         <v>781</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>172</v>
+        <v>66</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>61</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B10" s="128" t="s">
+        <v>783</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -5906,10 +5947,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2120DCC9-180B-41E9-8F7B-73DDDD34F142}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5922,13 +5963,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="29" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="130" t="s">
+      <c r="A1" s="132" t="s">
         <v>688</v>
       </c>
-      <c r="B1" s="131"/>
-      <c r="C1" s="131"/>
-      <c r="D1" s="131"/>
-      <c r="E1" s="132"/>
+      <c r="B1" s="133"/>
+      <c r="C1" s="133"/>
+      <c r="D1" s="133"/>
+      <c r="E1" s="134"/>
     </row>
     <row r="2" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="69" t="s">
@@ -5977,6 +6018,14 @@
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>776</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="135" t="s">
+        <v>791</v>
+      </c>
+      <c r="B9" t="s">
+        <v>792</v>
       </c>
     </row>
   </sheetData>
@@ -5992,7 +6041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F95DBB38-CB29-429B-8643-7E9E0FC99A14}">
   <dimension ref="A1:U35"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+    <sheetView topLeftCell="A21" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <selection activeCell="I20" sqref="I20:M22"/>
     </sheetView>
   </sheetViews>
@@ -6021,20 +6070,20 @@
       <c r="E1" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="I1" s="127" t="s">
+      <c r="I1" s="129" t="s">
         <v>496</v>
       </c>
-      <c r="J1" s="128"/>
-      <c r="K1" s="128"/>
-      <c r="L1" s="128"/>
-      <c r="M1" s="129"/>
-      <c r="Q1" s="127" t="s">
+      <c r="J1" s="130"/>
+      <c r="K1" s="130"/>
+      <c r="L1" s="130"/>
+      <c r="M1" s="131"/>
+      <c r="Q1" s="129" t="s">
         <v>499</v>
       </c>
-      <c r="R1" s="128"/>
-      <c r="S1" s="128"/>
-      <c r="T1" s="128"/>
-      <c r="U1" s="129"/>
+      <c r="R1" s="130"/>
+      <c r="S1" s="130"/>
+      <c r="T1" s="130"/>
+      <c r="U1" s="131"/>
     </row>
     <row r="2" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8">
@@ -6448,13 +6497,13 @@
       <c r="M17" s="12"/>
     </row>
     <row r="18" spans="1:13" ht="16" x14ac:dyDescent="0.4">
-      <c r="A18" s="127" t="s">
+      <c r="A18" s="129" t="s">
         <v>739</v>
       </c>
-      <c r="B18" s="128"/>
-      <c r="C18" s="128"/>
-      <c r="D18" s="128"/>
-      <c r="E18" s="129"/>
+      <c r="B18" s="130"/>
+      <c r="C18" s="130"/>
+      <c r="D18" s="130"/>
+      <c r="E18" s="131"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="8" t="s">
@@ -6740,10 +6789,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AD70"/>
+  <dimension ref="A1:AD74"/>
   <sheetViews>
-    <sheetView topLeftCell="F50" workbookViewId="0">
-      <selection activeCell="H64" sqref="H64"/>
+    <sheetView tabSelected="1" topLeftCell="C64" workbookViewId="0">
+      <selection activeCell="F75" sqref="F75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8684,6 +8733,49 @@
       <c r="M70" s="77" t="s">
         <v>42</v>
       </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A72" s="117" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" s="69" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="69" t="s">
+        <v>784</v>
+      </c>
+      <c r="B73" s="69" t="s">
+        <v>786</v>
+      </c>
+      <c r="C73" s="69" t="s">
+        <v>788</v>
+      </c>
+      <c r="D73" s="69" t="s">
+        <v>789</v>
+      </c>
+      <c r="E73" s="69" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" s="69" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="75" t="s">
+        <v>785</v>
+      </c>
+      <c r="B74" s="75" t="s">
+        <v>787</v>
+      </c>
+      <c r="C74" s="75" t="s">
+        <v>753</v>
+      </c>
+      <c r="D74" s="74" t="s">
+        <v>790</v>
+      </c>
+      <c r="E74" s="74" t="s">
+        <v>785</v>
+      </c>
+      <c r="I74" s="74"/>
+      <c r="J74" s="74"/>
+      <c r="L74" s="74"/>
+      <c r="M74" s="77"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -16481,7 +16573,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6D13D71-B365-458F-8758-84786862308D}">
   <dimension ref="A1:G82"/>
   <sheetViews>
-    <sheetView topLeftCell="A72" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A80" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>

</xml_diff>